<commit_message>
Matlab code clean-up, tutorial PDF
</commit_message>
<xml_diff>
--- a/participation_ratios.xlsx
+++ b/participation_ratios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>IBM_ratio_default</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Wang_Yale_DRIE_ratio</t>
-  </si>
-  <si>
-    <t>Wang_Yale_capacitance_leads</t>
   </si>
 </sst>
 </file>
@@ -439,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="G10" sqref="G10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +453,7 @@
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -478,11 +475,8 @@
       <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -507,11 +501,8 @@
       <c r="I2" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="K2" s="1">
-        <v>7.8800000000000002E-14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -536,11 +527,8 @@
       <c r="I3">
         <v>14.14</v>
       </c>
-      <c r="K3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -566,7 +554,7 @@
         <v>5.9982E-12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -592,7 +580,7 @@
         <v>4.2444E-16</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -618,7 +606,7 @@
         <v>3.3599E-15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -644,7 +632,7 @@
         <v>1.0892E-15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -670,7 +658,7 @@
         <v>7.0760999999999996E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -696,7 +684,7 @@
         <v>5.6015000000000004E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
IBM capacitance plots, update excel
</commit_message>
<xml_diff>
--- a/participation_ratios.xlsx
+++ b/participation_ratios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ratios" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>IBM_ratio_default</t>
   </si>
@@ -172,13 +172,25 @@
   </si>
   <si>
     <t>Yale_ratio_5fingers_rounded_r5_g_20um_l56</t>
+  </si>
+  <si>
+    <t>IBM_capacitance_w450_l60_sep_5</t>
+  </si>
+  <si>
+    <t>IBM_capacitance_w450_l60_sep_10</t>
+  </si>
+  <si>
+    <t>IBM_capacitance_w450_l60_sep_20</t>
+  </si>
+  <si>
+    <t>IBM_capacitance_w450_l60_sep_50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,25 +198,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -216,17 +216,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -818,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,10 +953,10 @@
       <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="2">
-        <v>14.14</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="B22">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C22">
         <v>6.5612000000000004</v>
       </c>
     </row>
@@ -978,8 +975,12 @@
       <c r="A24" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="B24">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C24">
+        <v>6.6116000000000001</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1034,15 +1035,23 @@
       <c r="A32" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="B32">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C32">
+        <v>6.5019999999999998</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="B33">
+        <v>14.141500000000001</v>
+      </c>
+      <c r="C33">
+        <v>6.5031999999999996</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1064,15 +1073,23 @@
       <c r="A37" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="B37">
+        <v>14.1411</v>
+      </c>
+      <c r="C37">
+        <v>6.5712000000000002</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="B38">
+        <v>14.1412</v>
+      </c>
+      <c r="C38">
+        <v>6.5784000000000002</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1092,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,6 +1160,38 @@
         <v>5.9400000000000004E-14</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8.0647E-14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7.0170000000000005E-14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6.0391000000000005E-14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.9340000000000001E-14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Calculated ratios, excel update
</commit_message>
<xml_diff>
--- a/participation_ratios.xlsx
+++ b/participation_ratios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ratios" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>IBM_ratio_default</t>
   </si>
@@ -123,12 +123,6 @@
     <t>Corrected Capacitances</t>
   </si>
   <si>
-    <t>Voltage</t>
-  </si>
-  <si>
-    <t>F0</t>
-  </si>
-  <si>
     <t>Yale_ratio_5fingers_rounded_g_20um_l56</t>
   </si>
   <si>
@@ -138,15 +132,6 @@
     <t>Slot Size</t>
   </si>
   <si>
-    <t>Yale_capacitance_5fingers_rounded_g_20um_l56_slot_10</t>
-  </si>
-  <si>
-    <t>Yale_capacitance_5fingers_rounded_g_20um_l56_slot_20</t>
-  </si>
-  <si>
-    <t>Yale_capacitance_5fingers_rounded_g_20um_l56_slot_50</t>
-  </si>
-  <si>
     <t>Corner radius</t>
   </si>
   <si>
@@ -184,13 +169,67 @@
   </si>
   <si>
     <t>IBM_capacitance_w450_l60_sep_50</t>
+  </si>
+  <si>
+    <t>Pma</t>
+  </si>
+  <si>
+    <t>Pms</t>
+  </si>
+  <si>
+    <t>Psa</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Yale_ratio_5fingers_rounded_g_20um_l56_slot_10</t>
+  </si>
+  <si>
+    <t>Yale_ratio_5fingers_rounded_g_20um_l56_slot_20</t>
+  </si>
+  <si>
+    <t>Yale_ratio_5fingers_rounded_g_20um_l56_slot_50</t>
+  </si>
+  <si>
+    <t>Relevant Parameters</t>
+  </si>
+  <si>
+    <t>#Fingers</t>
+  </si>
+  <si>
+    <t>Finger length [um]</t>
+  </si>
+  <si>
+    <t>Finger width = gap width [um]</t>
+  </si>
+  <si>
+    <t>Separation to ground [um]</t>
+  </si>
+  <si>
+    <t>Corner radius of fingers [um]</t>
+  </si>
+  <si>
+    <t>Resonance Frequency [GHz]</t>
+  </si>
+  <si>
+    <t>Capacitance [F]</t>
+  </si>
+  <si>
+    <t>Voltage over inductor [V]</t>
+  </si>
+  <si>
+    <t>P all (ma+ms+sa)</t>
+  </si>
+  <si>
+    <t>IBM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,16 +237,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -215,15 +308,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="11" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="11" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
+    <cellStyle name="60% - Accent5" xfId="4" builtinId="48"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -523,24 +641,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="3" width="17" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="29.42578125" customWidth="1"/>
     <col min="8" max="8" width="26.140625" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" customWidth="1"/>
+    <col min="12" max="12" width="45.85546875" customWidth="1"/>
+    <col min="13" max="14" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -565,8 +687,23 @@
       <c r="K1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -594,8 +731,23 @@
       <c r="K2" s="1">
         <v>7.8800000000000002E-14</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="M2" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="N2" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="O2" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="P2" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -623,8 +775,23 @@
       <c r="K3">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>14.1411</v>
+      </c>
+      <c r="M3">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="N3">
+        <v>14.14</v>
+      </c>
+      <c r="O3">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="P3">
+        <v>14.14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -649,8 +816,11 @@
       <c r="I4" s="1">
         <v>5.9982E-12</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="1">
+        <v>5.9991000000000002E-12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -675,8 +845,11 @@
       <c r="I5" s="1">
         <v>4.2444E-16</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="1">
+        <v>1.1104000000000001E-15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -701,8 +874,11 @@
       <c r="I6" s="1">
         <v>3.3599E-15</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="1">
+        <v>9.6884999999999996E-15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -727,8 +903,11 @@
       <c r="I7" s="1">
         <v>1.0892E-15</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="1">
+        <v>2.9612000000000001E-15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -753,8 +932,23 @@
       <c r="I8" s="1">
         <v>7.0760999999999996E-5</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="1">
+        <v>1.851E-4</v>
+      </c>
+      <c r="M8" s="1">
+        <v>8.6194999999999997E-5</v>
+      </c>
+      <c r="N8" s="1">
+        <v>5.0957E-5</v>
+      </c>
+      <c r="O8" s="1">
+        <v>1.3553999999999999E-4</v>
+      </c>
+      <c r="P8" s="1">
+        <v>7.5575999999999996E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -779,8 +973,23 @@
       <c r="I9" s="1">
         <v>5.6015000000000004E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="M9" s="1">
+        <v>8.4548999999999996E-4</v>
+      </c>
+      <c r="N9" s="1">
+        <v>5.1272999999999998E-4</v>
+      </c>
+      <c r="O9" s="1">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="P9" s="1">
+        <v>7.3333000000000003E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -804,6 +1013,21 @@
       </c>
       <c r="I10" s="1">
         <v>1.8159E-4</v>
+      </c>
+      <c r="L10" s="1">
+        <v>4.9359999999999996E-4</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2.6585999999999998E-4</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1.6066E-4</v>
+      </c>
+      <c r="O10" s="1">
+        <v>40.1235</v>
+      </c>
+      <c r="P10" s="1">
+        <v>2.4617999999999998E-4</v>
       </c>
     </row>
   </sheetData>
@@ -813,17 +1037,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="25" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -919,7 +1151,7 @@
         <v>13.95</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -927,183 +1159,824 @@
         <v>14.14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B20" t="s">
+      <c r="I21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>14.1411</v>
+      </c>
+      <c r="C22">
+        <v>6.5469999999999997</v>
+      </c>
+      <c r="D22" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.851E-4</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="G22" s="1">
+        <v>4.9359999999999996E-4</v>
+      </c>
+      <c r="H22" s="1">
+        <f>SUM(E22:G22)</f>
+        <v>2.2786999999999998E-3</v>
+      </c>
+      <c r="I22" s="2">
+        <v>5</v>
+      </c>
+      <c r="J22" s="4">
+        <v>5</v>
+      </c>
+      <c r="K22" s="4">
+        <v>87</v>
+      </c>
+      <c r="L22">
+        <v>20</v>
+      </c>
+      <c r="M22">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C23">
+        <v>6.5612000000000004</v>
+      </c>
+      <c r="D23" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="E23" s="1">
+        <v>8.6194999999999997E-5</v>
+      </c>
+      <c r="F23" s="1">
+        <v>8.4548999999999996E-4</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2.6585999999999998E-4</v>
+      </c>
+      <c r="H23" s="1">
+        <f>SUM(E23:G23)</f>
+        <v>1.1975449999999999E-3</v>
+      </c>
+      <c r="I23" s="2">
+        <v>5</v>
+      </c>
+      <c r="J23" s="4">
+        <v>10</v>
+      </c>
+      <c r="K23" s="4">
+        <v>76</v>
+      </c>
+      <c r="L23">
+        <v>20</v>
+      </c>
+      <c r="M23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="C20" t="s">
+      <c r="B24">
+        <v>14.14</v>
+      </c>
+      <c r="C24">
+        <v>6.5309999999999997</v>
+      </c>
+      <c r="D24" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="E24" s="7">
+        <v>5.0957E-5</v>
+      </c>
+      <c r="F24" s="7">
+        <v>5.1272999999999998E-4</v>
+      </c>
+      <c r="G24" s="7">
+        <v>1.6066E-4</v>
+      </c>
+      <c r="H24" s="7">
+        <f>SUM(E24:G24)</f>
+        <v>7.2434699999999997E-4</v>
+      </c>
+      <c r="I24" s="2">
+        <v>5</v>
+      </c>
+      <c r="J24" s="4">
+        <v>20</v>
+      </c>
+      <c r="K24" s="4">
+        <v>56</v>
+      </c>
+      <c r="L24">
+        <v>20</v>
+      </c>
+      <c r="M24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C25">
+        <v>6.6116000000000001</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1.3553999999999999E-4</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="G25" s="1">
+        <v>4.1235000000000002E-4</v>
+      </c>
+      <c r="H25" s="1">
+        <f>SUM(E25:G25)</f>
+        <v>1.84789E-3</v>
+      </c>
+      <c r="I25" s="2">
+        <v>10</v>
+      </c>
+      <c r="J25" s="4">
+        <v>5</v>
+      </c>
+      <c r="K25" s="4">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21">
-        <v>14.1411</v>
-      </c>
-      <c r="C21">
-        <v>6.5469999999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22">
+      <c r="L25">
+        <v>20</v>
+      </c>
+      <c r="M25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26">
+        <v>14.14</v>
+      </c>
+      <c r="C26">
+        <v>6.5195999999999996</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="E26" s="1">
+        <v>7.5575999999999996E-5</v>
+      </c>
+      <c r="F26" s="1">
+        <v>7.3333000000000003E-4</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2.4617999999999998E-4</v>
+      </c>
+      <c r="H26" s="1">
+        <f>SUM(E26:G26)</f>
+        <v>1.055086E-3</v>
+      </c>
+      <c r="I26" s="2">
+        <v>10</v>
+      </c>
+      <c r="J26" s="4">
+        <v>10</v>
+      </c>
+      <c r="K26" s="4">
+        <v>26</v>
+      </c>
+      <c r="L26">
+        <v>20</v>
+      </c>
+      <c r="M26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C30">
+        <v>6.5044000000000004</v>
+      </c>
+      <c r="D30" s="1">
+        <v>6.3499999999999994E-14</v>
+      </c>
+      <c r="E30" s="1">
+        <v>5.7122E-5</v>
+      </c>
+      <c r="F30" s="1">
+        <v>5.3123000000000005E-4</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1.784E-4</v>
+      </c>
+      <c r="H30" s="1">
+        <f>SUM(E30:G30)</f>
+        <v>7.667520000000001E-4</v>
+      </c>
+      <c r="I30" s="2">
+        <v>5</v>
+      </c>
+      <c r="J30" s="2">
+        <v>20</v>
+      </c>
+      <c r="K30" s="2">
+        <v>56</v>
+      </c>
+      <c r="L30" s="3">
+        <v>10</v>
+      </c>
+      <c r="M30" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31">
         <v>14.141299999999999</v>
       </c>
-      <c r="C22">
-        <v>6.5612000000000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23">
-        <v>14.14</v>
-      </c>
-      <c r="C23">
-        <v>6.5309999999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24">
-        <v>14.141400000000001</v>
-      </c>
-      <c r="C24">
-        <v>6.6116000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25">
-        <v>14.14</v>
-      </c>
-      <c r="C25">
-        <v>6.5195999999999996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29">
-        <v>14.141400000000001</v>
-      </c>
-      <c r="C29">
-        <v>6.5044000000000004</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30">
-        <v>14.141299999999999</v>
-      </c>
-      <c r="C30">
+      <c r="C31">
         <v>6.5035999999999996</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31">
-        <v>14.141400000000001</v>
-      </c>
-      <c r="C31">
-        <v>6.5044000000000004</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="1">
+        <v>5.9700000000000001E-14</v>
+      </c>
+      <c r="E31" s="7">
+        <v>6.1889000000000003E-5</v>
+      </c>
+      <c r="F31" s="7">
+        <v>5.4920000000000001E-4</v>
+      </c>
+      <c r="G31" s="7">
+        <v>1.7187999999999999E-4</v>
+      </c>
+      <c r="H31" s="7">
+        <f>SUM(E31:G31)</f>
+        <v>7.82969E-4</v>
+      </c>
+      <c r="I31" s="2">
+        <v>5</v>
+      </c>
+      <c r="J31" s="2">
+        <v>20</v>
+      </c>
+      <c r="K31" s="2">
+        <v>56</v>
+      </c>
+      <c r="L31" s="3">
+        <v>20</v>
+      </c>
+      <c r="M31" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B32">
         <v>14.141400000000001</v>
       </c>
       <c r="C32">
+        <v>6.5044000000000004</v>
+      </c>
+      <c r="D32" s="1">
+        <v>5.6800000000000002E-14</v>
+      </c>
+      <c r="E32" s="1">
+        <v>5.2184E-5</v>
+      </c>
+      <c r="F32" s="1">
+        <v>5.0383999999999997E-4</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1.6097E-4</v>
+      </c>
+      <c r="H32" s="1">
+        <f>SUM(E32:G32)</f>
+        <v>7.1699399999999999E-4</v>
+      </c>
+      <c r="I32" s="2">
+        <v>5</v>
+      </c>
+      <c r="J32" s="2">
+        <v>20</v>
+      </c>
+      <c r="K32" s="2">
+        <v>56</v>
+      </c>
+      <c r="L32" s="3">
+        <v>50</v>
+      </c>
+      <c r="M32" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C33">
         <v>6.5019999999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33">
+      <c r="D33" s="1">
+        <v>5.58E-14</v>
+      </c>
+      <c r="E33" s="1">
+        <v>4.8152000000000002E-5</v>
+      </c>
+      <c r="F33" s="1">
+        <v>4.9222000000000003E-4</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1.5393000000000001E-4</v>
+      </c>
+      <c r="H33" s="1">
+        <f>SUM(E33:G33)</f>
+        <v>6.9430200000000005E-4</v>
+      </c>
+      <c r="I33" s="2">
+        <v>5</v>
+      </c>
+      <c r="J33" s="2">
+        <v>20</v>
+      </c>
+      <c r="K33" s="2">
+        <v>56</v>
+      </c>
+      <c r="L33" s="3">
+        <v>100</v>
+      </c>
+      <c r="M33" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34">
         <v>14.141500000000001</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>6.5031999999999996</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36">
+      <c r="D34" s="1">
+        <v>5.5400000000000002E-14</v>
+      </c>
+      <c r="E34" s="1">
+        <v>5.0986000000000003E-5</v>
+      </c>
+      <c r="F34" s="1">
+        <v>4.8979999999999998E-4</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1.5875000000000001E-4</v>
+      </c>
+      <c r="H34" s="1">
+        <f>SUM(E34:G34)</f>
+        <v>6.9953600000000006E-4</v>
+      </c>
+      <c r="I34" s="2">
+        <v>5</v>
+      </c>
+      <c r="J34" s="2">
+        <v>20</v>
+      </c>
+      <c r="K34" s="2">
+        <v>56</v>
+      </c>
+      <c r="L34" s="3">
+        <v>200</v>
+      </c>
+      <c r="M34" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
         <v>14.141400000000001</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>6.5743999999999998</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37">
+      <c r="D37" s="1">
+        <v>6.1700000000000005E-14</v>
+      </c>
+      <c r="E37" s="7">
+        <v>5.1010000000000001E-5</v>
+      </c>
+      <c r="F37" s="7">
+        <v>5.3839000000000003E-4</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1.7016000000000001E-4</v>
+      </c>
+      <c r="H37" s="7">
+        <f>SUM(E37:G37)</f>
+        <v>7.5956000000000005E-4</v>
+      </c>
+      <c r="I37" s="2">
+        <v>5</v>
+      </c>
+      <c r="J37" s="2">
+        <v>20</v>
+      </c>
+      <c r="K37" s="2">
+        <v>56</v>
+      </c>
+      <c r="L37">
+        <v>20</v>
+      </c>
+      <c r="M37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
         <v>14.1411</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>6.5712000000000002</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38">
+      <c r="D38" s="1">
+        <v>6.1700000000000005E-14</v>
+      </c>
+      <c r="E38" s="1">
+        <v>6.5668999999999998E-5</v>
+      </c>
+      <c r="F38" s="1">
+        <v>5.9962999999999998E-4</v>
+      </c>
+      <c r="G38" s="1">
+        <v>1.8195E-4</v>
+      </c>
+      <c r="H38" s="1">
+        <f>SUM(E38:G38)</f>
+        <v>8.4724900000000001E-4</v>
+      </c>
+      <c r="I38" s="2">
+        <v>5</v>
+      </c>
+      <c r="J38" s="2">
+        <v>20</v>
+      </c>
+      <c r="K38" s="2">
+        <v>56</v>
+      </c>
+      <c r="L38">
+        <v>20</v>
+      </c>
+      <c r="M38" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39">
         <v>14.1412</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <v>6.5784000000000002</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39">
+      <c r="D39" s="1">
+        <v>6.1500000000000003E-14</v>
+      </c>
+      <c r="E39" s="1">
+        <v>6.6193999999999997E-5</v>
+      </c>
+      <c r="F39" s="1">
+        <v>5.7569000000000001E-4</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1.7843000000000001E-4</v>
+      </c>
+      <c r="H39" s="1">
+        <f>SUM(E39:G39)</f>
+        <v>8.2031400000000005E-4</v>
+      </c>
+      <c r="I39" s="2">
+        <v>5</v>
+      </c>
+      <c r="J39" s="2">
+        <v>20</v>
+      </c>
+      <c r="K39" s="2">
+        <v>56</v>
+      </c>
+      <c r="L39">
+        <v>20</v>
+      </c>
+      <c r="M39" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40">
         <v>14.141400000000001</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>6.4984000000000002</v>
       </c>
+      <c r="D40" s="1">
+        <v>5.9700000000000001E-14</v>
+      </c>
+      <c r="E40" s="1">
+        <v>5.0727999999999999E-5</v>
+      </c>
+      <c r="F40" s="1">
+        <v>5.2514E-4</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1.6347000000000001E-4</v>
+      </c>
+      <c r="H40" s="1">
+        <f>SUM(E40:G40)</f>
+        <v>7.3933799999999997E-4</v>
+      </c>
+      <c r="I40" s="2">
+        <v>5</v>
+      </c>
+      <c r="J40" s="2">
+        <v>20</v>
+      </c>
+      <c r="K40" s="2">
+        <v>56</v>
+      </c>
+      <c r="L40">
+        <v>20</v>
+      </c>
+      <c r="M40" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="M41" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D42" s="1"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43">
+        <v>14.14</v>
+      </c>
+      <c r="C43">
+        <v>6.5380000000000003</v>
+      </c>
+      <c r="D43" s="1">
+        <v>7.8800000000000002E-14</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1.2299E-5</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1.0498E-4</v>
+      </c>
+      <c r="G43" s="1">
+        <v>3.3423000000000002E-5</v>
+      </c>
+      <c r="H43" s="1">
+        <f>SUM(E43:G43)</f>
+        <v>1.5070200000000001E-4</v>
+      </c>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>14.14</v>
+      </c>
+      <c r="D45" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1.8599999999999999E-4</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="G45" s="1">
+        <v>4.9399999999999997E-4</v>
+      </c>
+      <c r="H45" s="1">
+        <f>SUM(E45:G45)</f>
+        <v>2.2799999999999999E-3</v>
+      </c>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>14.14</v>
+      </c>
+      <c r="D46" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1.0895000000000001E-4</v>
+      </c>
+      <c r="F46" s="1">
+        <v>9.7369999999999998E-4</v>
+      </c>
+      <c r="G46" s="1">
+        <v>2.9263999999999999E-4</v>
+      </c>
+      <c r="H46" s="1">
+        <f>SUM(E46:G46)</f>
+        <v>1.3752899999999999E-3</v>
+      </c>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47">
+        <v>14.14</v>
+      </c>
+      <c r="D47" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="E47" s="1">
+        <v>7.0760999999999996E-5</v>
+      </c>
+      <c r="F47" s="1">
+        <v>5.6015000000000004E-4</v>
+      </c>
+      <c r="G47" s="1">
+        <v>1.8159E-4</v>
+      </c>
+      <c r="H47" s="1">
+        <f>SUM(E47:G47)</f>
+        <v>8.1250100000000009E-4</v>
+      </c>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1111,8 +1984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,7 +2035,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1">
         <v>8.0647E-14</v>
@@ -1170,7 +2043,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1">
         <v>7.0170000000000005E-14</v>
@@ -1178,7 +2051,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1">
         <v>6.0391000000000005E-14</v>
@@ -1186,7 +2059,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1">
         <v>4.9340000000000001E-14</v>

</xml_diff>

<commit_message>
IBM ratios, updated excel
</commit_message>
<xml_diff>
--- a/participation_ratios.xlsx
+++ b/participation_ratios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="139">
   <si>
     <t>IBM_ratio_default</t>
   </si>
@@ -223,6 +223,216 @@
   </si>
   <si>
     <t>IBM</t>
+  </si>
+  <si>
+    <t>IBM_capacitance_w450_l60_sep_18_cornerr_sweep</t>
+  </si>
+  <si>
+    <t>r=5</t>
+  </si>
+  <si>
+    <t>r=10</t>
+  </si>
+  <si>
+    <t>r=15</t>
+  </si>
+  <si>
+    <t>r=20</t>
+  </si>
+  <si>
+    <t>r=25</t>
+  </si>
+  <si>
+    <t>r=29</t>
+  </si>
+  <si>
+    <t>IBM_capacitance_w450_s18_slotsize_650_padl_10_100</t>
+  </si>
+  <si>
+    <t>l=10</t>
+  </si>
+  <si>
+    <t>l=20</t>
+  </si>
+  <si>
+    <t>l=30</t>
+  </si>
+  <si>
+    <t>l=40</t>
+  </si>
+  <si>
+    <t>l=50</t>
+  </si>
+  <si>
+    <t>l=60</t>
+  </si>
+  <si>
+    <t>l=70</t>
+  </si>
+  <si>
+    <t>l=80</t>
+  </si>
+  <si>
+    <t>l=90</t>
+  </si>
+  <si>
+    <t>l=100</t>
+  </si>
+  <si>
+    <t>IBM_capacitance_w450_s18_slotsize_800_padl_10_100</t>
+  </si>
+  <si>
+    <t>IBM_capacitance_w450_l60_sep_sweep10_40</t>
+  </si>
+  <si>
+    <t>s=5</t>
+  </si>
+  <si>
+    <t>s=10</t>
+  </si>
+  <si>
+    <t>s=15</t>
+  </si>
+  <si>
+    <t>s=20</t>
+  </si>
+  <si>
+    <t>s=25</t>
+  </si>
+  <si>
+    <t>s=30</t>
+  </si>
+  <si>
+    <t>s=35</t>
+  </si>
+  <si>
+    <t>s=40</t>
+  </si>
+  <si>
+    <t>s=45</t>
+  </si>
+  <si>
+    <t>s=50</t>
+  </si>
+  <si>
+    <t>s=55</t>
+  </si>
+  <si>
+    <t>s=60</t>
+  </si>
+  <si>
+    <t>IBM_capacitance_w450_l60_s18_slotsize_500_800</t>
+  </si>
+  <si>
+    <t>slot_edge=500</t>
+  </si>
+  <si>
+    <t>slot_edge=533.333</t>
+  </si>
+  <si>
+    <t>slot_edge=566.667</t>
+  </si>
+  <si>
+    <t>slot_edge=600</t>
+  </si>
+  <si>
+    <t>slot_edge=633.333</t>
+  </si>
+  <si>
+    <t>slot_edge=666.667</t>
+  </si>
+  <si>
+    <t>slot_edge=700</t>
+  </si>
+  <si>
+    <t>slot_edge=733.333</t>
+  </si>
+  <si>
+    <t>slot_edge=766.667</t>
+  </si>
+  <si>
+    <t>slot_edge=800</t>
+  </si>
+  <si>
+    <t>IBM_capacitance_w450_l60_sep_18</t>
+  </si>
+  <si>
+    <t>pad_w=300</t>
+  </si>
+  <si>
+    <t>pad_w=325</t>
+  </si>
+  <si>
+    <t>pad_w=350</t>
+  </si>
+  <si>
+    <t>pad_w=375</t>
+  </si>
+  <si>
+    <t>pad_w=400</t>
+  </si>
+  <si>
+    <t>pad_w=425</t>
+  </si>
+  <si>
+    <t>pad_w=450</t>
+  </si>
+  <si>
+    <t>pad_w=475</t>
+  </si>
+  <si>
+    <t>pad_w=500</t>
+  </si>
+  <si>
+    <t>IBM_fixed_slot_sweep_w300_500</t>
+  </si>
+  <si>
+    <t>Resonance Frequency</t>
+  </si>
+  <si>
+    <t>Target Capacitance</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_sep_5</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_sep_10</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_sep_20</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_sep_50</t>
+  </si>
+  <si>
+    <t>Pad Width [um]</t>
+  </si>
+  <si>
+    <t>Pad Separation</t>
+  </si>
+  <si>
+    <t>Pad Separation [um]</t>
+  </si>
+  <si>
+    <t>Pad Length [um]</t>
+  </si>
+  <si>
+    <t>Corner radius of pads [um]</t>
+  </si>
+  <si>
+    <t>#Mesh elements</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Slot size [um]</t>
+  </si>
+  <si>
+    <t>Yale</t>
+  </si>
+  <si>
+    <t>Inductance [H]</t>
   </si>
 </sst>
 </file>
@@ -275,7 +485,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +509,11 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -318,14 +533,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -336,10 +552,13 @@
     <xf numFmtId="11" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4"/>
     <xf numFmtId="11" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
     <cellStyle name="60% - Accent5" xfId="4" builtinId="48"/>
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1037,41 +1256,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A16" sqref="A16"/>
+      <selection pane="topRight" activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="13" max="13" width="26.28515625" customWidth="1"/>
+    <col min="3" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="25" customWidth="1"/>
+    <col min="14" max="14" width="26.28515625" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1079,7 +1301,7 @@
         <v>14.14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1087,7 +1309,7 @@
         <v>14.14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1095,7 +1317,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1103,7 +1325,7 @@
         <v>14.14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1111,7 +1333,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1119,7 +1341,7 @@
         <v>14.14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1127,7 +1349,7 @@
         <v>14.14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1135,15 +1357,15 @@
         <v>14.14</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>13.97</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1151,7 +1373,7 @@
         <v>13.95</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1159,7 +1381,12 @@
         <v>14.14</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>54</v>
       </c>
@@ -1170,46 +1397,52 @@
         <v>64</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="I20" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="J20" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J20" s="6" t="s">
+      <c r="K20" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="L20" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L20" s="6" t="s">
+      <c r="M20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="N20" s="6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O20" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1220,38 +1453,44 @@
         <v>6.5469999999999997</v>
       </c>
       <c r="D22" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="E22" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>1.851E-4</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>4.9359999999999996E-4</v>
       </c>
-      <c r="H22" s="1">
-        <f>SUM(E22:G22)</f>
+      <c r="I22" s="1">
+        <f>SUM(F22:H22)</f>
         <v>2.2786999999999998E-3</v>
       </c>
-      <c r="I22" s="2">
+      <c r="J22" s="2">
         <v>5</v>
       </c>
-      <c r="J22" s="4">
+      <c r="K22" s="4">
         <v>5</v>
       </c>
-      <c r="K22" s="4">
+      <c r="L22" s="4">
         <v>87</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>20</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <v>1242502</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1262,38 +1501,44 @@
         <v>6.5612000000000004</v>
       </c>
       <c r="D23" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="E23" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>8.6194999999999997E-5</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>8.4548999999999996E-4</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>2.6585999999999998E-4</v>
       </c>
-      <c r="H23" s="1">
-        <f>SUM(E23:G23)</f>
+      <c r="I23" s="1">
+        <f>SUM(F23:H23)</f>
         <v>1.1975449999999999E-3</v>
       </c>
-      <c r="I23" s="2">
+      <c r="J23" s="2">
         <v>5</v>
       </c>
-      <c r="J23" s="4">
+      <c r="K23" s="4">
         <v>10</v>
       </c>
-      <c r="K23" s="4">
+      <c r="L23" s="4">
         <v>76</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>20</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <v>789156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1304,38 +1549,44 @@
         <v>6.5309999999999997</v>
       </c>
       <c r="D24" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="E24" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="E24" s="7">
+      <c r="F24" s="7">
         <v>5.0957E-5</v>
       </c>
-      <c r="F24" s="7">
+      <c r="G24" s="7">
         <v>5.1272999999999998E-4</v>
       </c>
-      <c r="G24" s="7">
+      <c r="H24" s="7">
         <v>1.6066E-4</v>
       </c>
-      <c r="H24" s="7">
-        <f>SUM(E24:G24)</f>
+      <c r="I24" s="7">
+        <f>SUM(F24:H24)</f>
         <v>7.2434699999999997E-4</v>
       </c>
-      <c r="I24" s="2">
+      <c r="J24" s="2">
         <v>5</v>
       </c>
-      <c r="J24" s="4">
+      <c r="K24" s="4">
         <v>20</v>
       </c>
-      <c r="K24" s="4">
+      <c r="L24" s="4">
         <v>56</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>20</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>688893</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1346,38 +1597,44 @@
         <v>6.6116000000000001</v>
       </c>
       <c r="D25" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="E25" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>1.3553999999999999E-4</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>4.1235000000000002E-4</v>
       </c>
-      <c r="H25" s="1">
-        <f>SUM(E25:G25)</f>
+      <c r="I25" s="1">
+        <f>SUM(F25:H25)</f>
         <v>1.84789E-3</v>
       </c>
-      <c r="I25" s="2">
+      <c r="J25" s="2">
         <v>10</v>
       </c>
-      <c r="J25" s="4">
+      <c r="K25" s="4">
         <v>5</v>
       </c>
-      <c r="K25" s="4">
+      <c r="L25" s="4">
         <v>36</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>20</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>660464</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1388,53 +1645,59 @@
         <v>6.5195999999999996</v>
       </c>
       <c r="D26" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="E26" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>7.5575999999999996E-5</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>7.3333000000000003E-4</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>2.4617999999999998E-4</v>
       </c>
-      <c r="H26" s="1">
-        <f>SUM(E26:G26)</f>
+      <c r="I26" s="1">
+        <f>SUM(F26:H26)</f>
         <v>1.055086E-3</v>
       </c>
-      <c r="I26" s="2">
+      <c r="J26" s="2">
         <v>10</v>
       </c>
-      <c r="J26" s="4">
+      <c r="K26" s="4">
         <v>10</v>
       </c>
-      <c r="K26" s="4">
+      <c r="L26" s="4">
         <v>26</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>20</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I27" s="2"/>
+      <c r="O26">
+        <v>1051136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I28" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1444,39 +1707,42 @@
       <c r="C30">
         <v>6.5044000000000004</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>6.3499999999999994E-14</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>5.7122E-5</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>5.3123000000000005E-4</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>1.784E-4</v>
       </c>
-      <c r="H30" s="1">
-        <f>SUM(E30:G30)</f>
+      <c r="I30" s="1">
+        <f>SUM(F30:H30)</f>
         <v>7.667520000000001E-4</v>
       </c>
-      <c r="I30" s="2">
+      <c r="J30" s="2">
         <v>5</v>
       </c>
-      <c r="J30" s="2">
+      <c r="K30" s="2">
         <v>20</v>
       </c>
-      <c r="K30" s="2">
+      <c r="L30" s="2">
         <v>56</v>
       </c>
-      <c r="L30" s="3">
+      <c r="M30" s="3">
         <v>10</v>
       </c>
-      <c r="M30" s="2">
+      <c r="N30" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O30" s="2">
+        <v>702518</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1486,39 +1752,42 @@
       <c r="C31">
         <v>6.5035999999999996</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>5.9700000000000001E-14</v>
       </c>
-      <c r="E31" s="7">
+      <c r="F31" s="7">
         <v>6.1889000000000003E-5</v>
       </c>
-      <c r="F31" s="7">
+      <c r="G31" s="7">
         <v>5.4920000000000001E-4</v>
       </c>
-      <c r="G31" s="7">
+      <c r="H31" s="7">
         <v>1.7187999999999999E-4</v>
       </c>
-      <c r="H31" s="7">
-        <f>SUM(E31:G31)</f>
+      <c r="I31" s="7">
+        <f>SUM(F31:H31)</f>
         <v>7.82969E-4</v>
       </c>
-      <c r="I31" s="2">
+      <c r="J31" s="2">
         <v>5</v>
       </c>
-      <c r="J31" s="2">
+      <c r="K31" s="2">
         <v>20</v>
       </c>
-      <c r="K31" s="2">
+      <c r="L31" s="2">
         <v>56</v>
       </c>
-      <c r="L31" s="3">
+      <c r="M31" s="3">
         <v>20</v>
       </c>
-      <c r="M31" s="2">
+      <c r="N31" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O31" s="2">
+        <v>886630</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -1528,39 +1797,42 @@
       <c r="C32">
         <v>6.5044000000000004</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>5.6800000000000002E-14</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <v>5.2184E-5</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>5.0383999999999997E-4</v>
       </c>
-      <c r="G32" s="1">
+      <c r="H32" s="1">
         <v>1.6097E-4</v>
       </c>
-      <c r="H32" s="1">
-        <f>SUM(E32:G32)</f>
+      <c r="I32" s="1">
+        <f>SUM(F32:H32)</f>
         <v>7.1699399999999999E-4</v>
       </c>
-      <c r="I32" s="2">
+      <c r="J32" s="2">
         <v>5</v>
       </c>
-      <c r="J32" s="2">
+      <c r="K32" s="2">
         <v>20</v>
       </c>
-      <c r="K32" s="2">
+      <c r="L32" s="2">
         <v>56</v>
       </c>
-      <c r="L32" s="3">
+      <c r="M32" s="3">
         <v>50</v>
       </c>
-      <c r="M32" s="2">
+      <c r="N32" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O32" s="2">
+        <v>789245</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1570,39 +1842,42 @@
       <c r="C33">
         <v>6.5019999999999998</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>5.58E-14</v>
       </c>
-      <c r="E33" s="1">
+      <c r="F33" s="1">
         <v>4.8152000000000002E-5</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="1">
         <v>4.9222000000000003E-4</v>
       </c>
-      <c r="G33" s="1">
+      <c r="H33" s="1">
         <v>1.5393000000000001E-4</v>
       </c>
-      <c r="H33" s="1">
-        <f>SUM(E33:G33)</f>
+      <c r="I33" s="1">
+        <f>SUM(F33:H33)</f>
         <v>6.9430200000000005E-4</v>
       </c>
-      <c r="I33" s="2">
+      <c r="J33" s="2">
         <v>5</v>
       </c>
-      <c r="J33" s="2">
+      <c r="K33" s="2">
         <v>20</v>
       </c>
-      <c r="K33" s="2">
+      <c r="L33" s="2">
         <v>56</v>
       </c>
-      <c r="L33" s="3">
+      <c r="M33" s="3">
         <v>100</v>
       </c>
-      <c r="M33" s="2">
+      <c r="N33" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O33" s="2">
+        <v>670572</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1612,50 +1887,53 @@
       <c r="C34">
         <v>6.5031999999999996</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <v>5.5400000000000002E-14</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <v>5.0986000000000003E-5</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <v>4.8979999999999998E-4</v>
       </c>
-      <c r="G34" s="1">
+      <c r="H34" s="1">
         <v>1.5875000000000001E-4</v>
       </c>
-      <c r="H34" s="1">
-        <f>SUM(E34:G34)</f>
+      <c r="I34" s="1">
+        <f>SUM(F34:H34)</f>
         <v>6.9953600000000006E-4</v>
       </c>
-      <c r="I34" s="2">
+      <c r="J34" s="2">
         <v>5</v>
       </c>
-      <c r="J34" s="2">
+      <c r="K34" s="2">
         <v>20</v>
       </c>
-      <c r="K34" s="2">
+      <c r="L34" s="2">
         <v>56</v>
       </c>
-      <c r="L34" s="3">
+      <c r="M34" s="3">
         <v>200</v>
       </c>
-      <c r="M34" s="2">
+      <c r="N34" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I35" s="2"/>
+      <c r="O34" s="2">
+        <v>684785</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I36" s="2"/>
       <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1665,39 +1943,42 @@
       <c r="C37">
         <v>6.5743999999999998</v>
       </c>
-      <c r="D37" s="1">
+      <c r="E37" s="1">
         <v>6.1700000000000005E-14</v>
       </c>
-      <c r="E37" s="7">
+      <c r="F37" s="7">
         <v>5.1010000000000001E-5</v>
       </c>
-      <c r="F37" s="7">
+      <c r="G37" s="7">
         <v>5.3839000000000003E-4</v>
       </c>
-      <c r="G37" s="7">
+      <c r="H37" s="7">
         <v>1.7016000000000001E-4</v>
       </c>
-      <c r="H37" s="7">
-        <f>SUM(E37:G37)</f>
+      <c r="I37" s="7">
+        <f>SUM(F37:H37)</f>
         <v>7.5956000000000005E-4</v>
       </c>
-      <c r="I37" s="2">
+      <c r="J37" s="2">
         <v>5</v>
       </c>
-      <c r="J37" s="2">
+      <c r="K37" s="2">
         <v>20</v>
       </c>
-      <c r="K37" s="2">
+      <c r="L37" s="2">
         <v>56</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>20</v>
       </c>
-      <c r="M37" s="3">
+      <c r="N37" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O37" s="11">
+        <v>706509</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1707,39 +1988,42 @@
       <c r="C38">
         <v>6.5712000000000002</v>
       </c>
-      <c r="D38" s="1">
+      <c r="E38" s="1">
         <v>6.1700000000000005E-14</v>
       </c>
-      <c r="E38" s="1">
+      <c r="F38" s="1">
         <v>6.5668999999999998E-5</v>
       </c>
-      <c r="F38" s="1">
+      <c r="G38" s="1">
         <v>5.9962999999999998E-4</v>
       </c>
-      <c r="G38" s="1">
+      <c r="H38" s="1">
         <v>1.8195E-4</v>
       </c>
-      <c r="H38" s="1">
-        <f>SUM(E38:G38)</f>
+      <c r="I38" s="1">
+        <f>SUM(F38:H38)</f>
         <v>8.4724900000000001E-4</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>5</v>
       </c>
-      <c r="J38" s="2">
+      <c r="K38" s="2">
         <v>20</v>
       </c>
-      <c r="K38" s="2">
+      <c r="L38" s="2">
         <v>56</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <v>20</v>
       </c>
-      <c r="M38" s="3">
+      <c r="N38" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <v>1105979</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -1749,39 +2033,42 @@
       <c r="C39">
         <v>6.5784000000000002</v>
       </c>
-      <c r="D39" s="1">
+      <c r="E39" s="1">
         <v>6.1500000000000003E-14</v>
       </c>
-      <c r="E39" s="1">
+      <c r="F39" s="1">
         <v>6.6193999999999997E-5</v>
       </c>
-      <c r="F39" s="1">
+      <c r="G39" s="1">
         <v>5.7569000000000001E-4</v>
       </c>
-      <c r="G39" s="1">
+      <c r="H39" s="1">
         <v>1.7843000000000001E-4</v>
       </c>
-      <c r="H39" s="1">
-        <f>SUM(E39:G39)</f>
+      <c r="I39" s="1">
+        <f>SUM(F39:H39)</f>
         <v>8.2031400000000005E-4</v>
       </c>
-      <c r="I39" s="2">
+      <c r="J39" s="2">
         <v>5</v>
       </c>
-      <c r="J39" s="2">
+      <c r="K39" s="2">
         <v>20</v>
       </c>
-      <c r="K39" s="2">
+      <c r="L39" s="2">
         <v>56</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <v>20</v>
       </c>
-      <c r="M39" s="3">
+      <c r="N39" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <v>1194951</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1791,61 +2078,65 @@
       <c r="C40">
         <v>6.4984000000000002</v>
       </c>
-      <c r="D40" s="1">
+      <c r="E40" s="1">
         <v>5.9700000000000001E-14</v>
       </c>
-      <c r="E40" s="1">
+      <c r="F40" s="1">
         <v>5.0727999999999999E-5</v>
       </c>
-      <c r="F40" s="1">
+      <c r="G40" s="1">
         <v>5.2514E-4</v>
       </c>
-      <c r="G40" s="1">
+      <c r="H40" s="1">
         <v>1.6347000000000001E-4</v>
       </c>
-      <c r="H40" s="1">
-        <f>SUM(E40:G40)</f>
+      <c r="I40" s="1">
+        <f>SUM(F40:H40)</f>
         <v>7.3933799999999997E-4</v>
       </c>
-      <c r="I40" s="2">
+      <c r="J40" s="2">
         <v>5</v>
       </c>
-      <c r="J40" s="2">
+      <c r="K40" s="2">
         <v>20</v>
       </c>
-      <c r="K40" s="2">
+      <c r="L40" s="2">
         <v>56</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <v>20</v>
       </c>
-      <c r="M40" s="3">
+      <c r="N40" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O40" s="11">
+        <v>696744</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>56</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
+      <c r="D41" s="8"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
-      <c r="I41" s="2"/>
+      <c r="I41" s="9"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="M41" s="3">
+      <c r="L41" s="2"/>
+      <c r="N41" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D42" s="1"/>
-      <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E42" s="1"/>
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -1855,124 +2146,417 @@
       <c r="C43">
         <v>6.5380000000000003</v>
       </c>
-      <c r="D43" s="1">
+      <c r="E43" s="1">
         <v>7.8800000000000002E-14</v>
       </c>
-      <c r="E43" s="1">
+      <c r="F43" s="1">
         <v>1.2299E-5</v>
       </c>
-      <c r="F43" s="1">
+      <c r="G43" s="1">
         <v>1.0498E-4</v>
       </c>
-      <c r="G43" s="1">
+      <c r="H43" s="1">
         <v>3.3423000000000002E-5</v>
       </c>
-      <c r="H43" s="1">
-        <f>SUM(E43:G43)</f>
+      <c r="I43" s="1">
+        <f>SUM(F43:H43)</f>
         <v>1.5070200000000001E-4</v>
       </c>
-      <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J43" s="2"/>
+      <c r="O43">
+        <v>667194</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
       <c r="B45">
         <v>14.14</v>
       </c>
-      <c r="D45" s="1">
+      <c r="C45">
+        <v>6.55</v>
+      </c>
+      <c r="E45" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="E45" s="1">
+      <c r="F45" s="1">
         <v>1.8599999999999999E-4</v>
       </c>
-      <c r="F45" s="1">
+      <c r="G45" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="G45" s="1">
+      <c r="H45" s="1">
         <v>4.9399999999999997E-4</v>
       </c>
-      <c r="H45" s="1">
-        <f>SUM(E45:G45)</f>
+      <c r="I45" s="1">
+        <f>SUM(F45:H45)</f>
         <v>2.2799999999999999E-3</v>
       </c>
-      <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J45" s="2">
+        <v>5</v>
+      </c>
+      <c r="K45" s="2">
+        <v>5</v>
+      </c>
+      <c r="L45" s="2">
+        <v>86.9</v>
+      </c>
+      <c r="M45" s="2">
+        <v>20</v>
+      </c>
+      <c r="N45" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="O45" s="2">
+        <v>1247728</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>24</v>
       </c>
       <c r="B46">
         <v>14.14</v>
       </c>
-      <c r="D46" s="1">
+      <c r="C46">
+        <v>6.4939999999999998</v>
+      </c>
+      <c r="E46" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="E46" s="1">
+      <c r="F46" s="1">
         <v>1.0895000000000001E-4</v>
       </c>
-      <c r="F46" s="1">
+      <c r="G46" s="1">
         <v>9.7369999999999998E-4</v>
       </c>
-      <c r="G46" s="1">
+      <c r="H46" s="1">
         <v>2.9263999999999999E-4</v>
       </c>
-      <c r="H46" s="1">
-        <f>SUM(E46:G46)</f>
+      <c r="I46" s="1">
+        <f>SUM(F46:H46)</f>
         <v>1.3752899999999999E-3</v>
       </c>
-      <c r="I46" s="2"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J46" s="2">
+        <v>5</v>
+      </c>
+      <c r="K46" s="2">
+        <v>10</v>
+      </c>
+      <c r="L46" s="2">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="M46" s="2">
+        <v>20</v>
+      </c>
+      <c r="N46" s="2">
+        <v>5</v>
+      </c>
+      <c r="O46" s="2">
+        <v>1513610</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>22</v>
       </c>
       <c r="B47">
         <v>14.14</v>
       </c>
-      <c r="D47" s="1">
+      <c r="C47" s="11">
+        <v>6.6580000000000004</v>
+      </c>
+      <c r="E47" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="E47" s="1">
+      <c r="F47" s="1">
         <v>7.0760999999999996E-5</v>
       </c>
-      <c r="F47" s="1">
+      <c r="G47" s="1">
         <v>5.6015000000000004E-4</v>
       </c>
-      <c r="G47" s="1">
+      <c r="H47" s="1">
         <v>1.8159E-4</v>
       </c>
-      <c r="H47" s="1">
-        <f>SUM(E47:G47)</f>
+      <c r="I47" s="1">
+        <f>SUM(F47:H47)</f>
         <v>8.1250100000000009E-4</v>
       </c>
-      <c r="I47" s="2"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="J47" s="2">
+        <v>5</v>
+      </c>
+      <c r="K47" s="2">
+        <v>20</v>
+      </c>
+      <c r="L47" s="2">
+        <v>56.9</v>
+      </c>
+      <c r="M47" s="2">
+        <v>20</v>
+      </c>
+      <c r="N47" s="2">
+        <v>10</v>
+      </c>
+      <c r="O47" s="2">
+        <v>1373883</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
+    </row>
+    <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="M50" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="N50" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="O50" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B53" s="1">
+        <v>14.141</v>
+      </c>
+      <c r="C53">
+        <v>6.5072000000000001</v>
+      </c>
+      <c r="E53" s="1">
+        <v>8.0647E-14</v>
+      </c>
+      <c r="F53" s="1">
+        <v>6.4206000000000002E-5</v>
+      </c>
+      <c r="G53" s="1">
+        <v>5.9539E-4</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1.8191999999999999E-4</v>
+      </c>
+      <c r="I53" s="1">
+        <f>SUM(F53:H53)</f>
+        <v>8.4151600000000005E-4</v>
+      </c>
+      <c r="J53">
+        <v>450</v>
+      </c>
+      <c r="K53" s="3">
+        <v>5</v>
+      </c>
+      <c r="L53">
+        <v>60</v>
+      </c>
+      <c r="M53">
+        <v>650</v>
+      </c>
+      <c r="N53" t="s">
+        <v>135</v>
+      </c>
+      <c r="O53">
+        <v>934556</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" s="1">
+        <v>14.1411</v>
+      </c>
+      <c r="C54">
+        <v>6.5056000000000003</v>
+      </c>
+      <c r="E54" s="1">
+        <v>7.0170000000000005E-14</v>
+      </c>
+      <c r="F54" s="1">
+        <v>4.6547E-5</v>
+      </c>
+      <c r="G54" s="1">
+        <v>4.2583999999999998E-4</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1.2769999999999999E-4</v>
+      </c>
+      <c r="I54" s="1">
+        <f t="shared" ref="I54:I56" si="0">SUM(F54:H54)</f>
+        <v>6.0008700000000002E-4</v>
+      </c>
+      <c r="J54">
+        <v>450</v>
+      </c>
+      <c r="K54" s="3">
+        <v>10</v>
+      </c>
+      <c r="L54">
+        <v>60</v>
+      </c>
+      <c r="M54">
+        <v>650</v>
+      </c>
+      <c r="N54" t="s">
+        <v>135</v>
+      </c>
+      <c r="O54">
+        <v>995525</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C55">
+        <v>6.5044000000000004</v>
+      </c>
+      <c r="E55" s="1">
+        <v>6.0391000000000005E-14</v>
+      </c>
+      <c r="F55" s="1">
+        <v>4.0198999999999999E-5</v>
+      </c>
+      <c r="G55" s="1">
+        <v>3.2086000000000001E-4</v>
+      </c>
+      <c r="H55" s="1">
+        <v>9.6681000000000005E-5</v>
+      </c>
+      <c r="I55" s="1">
+        <f t="shared" si="0"/>
+        <v>4.5773999999999999E-4</v>
+      </c>
+      <c r="J55">
+        <v>450</v>
+      </c>
+      <c r="K55" s="3">
+        <v>20</v>
+      </c>
+      <c r="L55">
+        <v>60</v>
+      </c>
+      <c r="M55">
+        <v>650</v>
+      </c>
+      <c r="N55" t="s">
+        <v>135</v>
+      </c>
+      <c r="O55">
+        <v>1041000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C56">
+        <v>6.5060000000000002</v>
+      </c>
+      <c r="E56" s="1">
+        <v>4.9340000000000001E-14</v>
+      </c>
+      <c r="F56" s="1">
+        <v>3.3513999999999998E-5</v>
+      </c>
+      <c r="G56" s="1">
+        <v>2.5494E-4</v>
+      </c>
+      <c r="H56" s="1">
+        <v>7.6984999999999996E-5</v>
+      </c>
+      <c r="I56" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6543900000000001E-4</v>
+      </c>
+      <c r="J56">
+        <v>450</v>
+      </c>
+      <c r="K56" s="3">
+        <v>50</v>
+      </c>
+      <c r="L56">
+        <v>60</v>
+      </c>
+      <c r="M56">
+        <v>650</v>
+      </c>
+      <c r="N56" t="s">
+        <v>135</v>
+      </c>
+      <c r="O56">
+        <v>1083873</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1982,87 +2566,1003 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="1">
+        <v>6500000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="C2" s="1">
+        <f>1/((2*PI()*$B$1)^2*B2)</f>
+        <v>9.992227183662502E-9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B3" s="1">
         <v>6.1700000000000005E-14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C66" si="0">1/((2*PI()*$B$1)^2*B3)</f>
+        <v>9.7169146032374405E-9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B4" s="1">
         <v>6.1700000000000005E-14</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>9.7169146032374405E-9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B5" s="1">
         <v>6.1500000000000003E-14</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>9.7485143255243924E-9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B6" s="1">
         <v>5.9700000000000001E-14</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.004243938056533E-8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B7" s="1">
         <v>5.9400000000000004E-14</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0093158771376264E-8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B9" s="1">
         <v>8.0647E-14</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>7.4340475283612555E-9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B10" s="1">
         <v>7.0170000000000005E-14</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>8.5440164033026945E-9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B11" s="1">
         <v>6.0391000000000005E-14</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>9.9275327618312342E-9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B12" s="1">
         <v>4.9340000000000001E-14</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2151066700846172E-8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="1">
+        <v>6.1720000000000001E-14</v>
+      </c>
+      <c r="C15" s="1">
+        <f>1/((2*PI()*$B$1)^2*B15)</f>
+        <v>9.713765894681629E-9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6.1463999999999997E-14</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>9.7542241152503943E-9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.1125899999999994E-14</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>9.8081767470049562E-9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="1">
+        <v>6.0706000000000002E-14</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>9.8760193559079859E-9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="1">
+        <v>6.0221000000000004E-14</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>9.9555575466988284E-9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="1">
+        <v>5.9773400000000001E-14</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0030107556534346E-8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="1">
+        <v>3.54973E-14</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6889555854100175E-8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4.3846300000000001E-14</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="0"/>
+        <v>1.367352846237311E-8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="1">
+        <v>4.9731000000000003E-14</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="0"/>
+        <v>1.205553137921518E-8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="1">
+        <v>5.4420699999999997E-14</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1016646809389628E-8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="1">
+        <v>5.83753E-14</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0270330619624226E-8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="1">
+        <v>6.1855399999999996E-14</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="0"/>
+        <v>9.6925026920810491E-9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="1">
+        <v>6.4977799999999997E-14</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="0"/>
+        <v>9.2267456118820612E-9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="1">
+        <v>6.7879099999999995E-14</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
+        <v>8.8323744866939921E-9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="1">
+        <v>7.0575300000000001E-14</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="0"/>
+        <v>8.4949498056650141E-9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="1">
+        <v>7.3130200000000002E-14</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" si="0"/>
+        <v>8.1981675288697437E-9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3.5513000000000001E-14</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6882089122849381E-8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="1">
+        <v>4.3856700000000003E-14</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3670285977279413E-8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="1">
+        <v>4.9696900000000002E-14</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2063803396585102E-8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="1">
+        <v>5.4334E-14</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="0"/>
+        <v>1.10342259178369E-8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="1">
+        <v>5.8308200000000002E-14</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="0"/>
+        <v>1.028214952647741E-8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="1">
+        <v>6.1670099999999998E-14</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="0"/>
+        <v>9.7216257314281987E-9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="1">
+        <v>6.4743099999999995E-14</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="0"/>
+        <v>9.2601934572139756E-9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="1">
+        <v>6.7543999999999995E-14</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="0"/>
+        <v>8.8761937554742127E-9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="1">
+        <v>7.0155300000000001E-14</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="0"/>
+        <v>8.5458066749019692E-9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="1">
+        <v>7.2587300000000003E-14</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="0"/>
+        <v>8.2594838355986524E-9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="1">
+        <v>8.0646599999999996E-14</v>
+      </c>
+      <c r="C47" s="1">
+        <f t="shared" si="0"/>
+        <v>7.4340844005791962E-9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="1">
+        <v>7.0201500000000001E-14</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="0"/>
+        <v>8.5401826317065899E-9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" s="1">
+        <v>6.4368000000000001E-14</v>
+      </c>
+      <c r="C49" s="1">
+        <f t="shared" si="0"/>
+        <v>9.3141565843237348E-9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="1">
+        <v>6.0415700000000001E-14</v>
+      </c>
+      <c r="C50" s="1">
+        <f t="shared" si="0"/>
+        <v>9.923474047635799E-9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="1">
+        <v>5.7484800000000005E-14</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0429428840663098E-8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" s="1">
+        <v>5.5171000000000003E-14</v>
+      </c>
+      <c r="C52" s="1">
+        <f t="shared" si="0"/>
+        <v>1.086682552463704E-8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>95</v>
+      </c>
+      <c r="B53" s="1">
+        <v>5.3318800000000002E-14</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1244319658727318E-8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="1">
+        <v>5.1764799999999999E-14</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1581878632193115E-8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="1">
+        <v>5.0462599999999999E-14</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1880751903781219E-8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="1">
+        <v>4.9338800000000003E-14</v>
+      </c>
+      <c r="C56" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2151362234585156E-8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" s="1">
+        <v>4.8364000000000001E-14</v>
+      </c>
+      <c r="C57" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2396278864852992E-8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>100</v>
+      </c>
+      <c r="B58" s="1">
+        <v>4.7512400000000001E-14</v>
+      </c>
+      <c r="C58" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2618466569143004E-8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61" s="1">
+        <v>6.2816899999999994E-14</v>
+      </c>
+      <c r="C61" s="1">
+        <f t="shared" si="0"/>
+        <v>9.544145461169688E-9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62" s="1">
+        <v>6.2381000000000005E-14</v>
+      </c>
+      <c r="C62" s="1">
+        <f t="shared" si="0"/>
+        <v>9.610837130211925E-9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" s="1">
+        <v>6.2144200000000002E-14</v>
+      </c>
+      <c r="C63" s="1">
+        <f t="shared" si="0"/>
+        <v>9.6474591517752274E-9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>105</v>
+      </c>
+      <c r="B64" s="1">
+        <v>6.2012900000000001E-14</v>
+      </c>
+      <c r="C64" s="1">
+        <f t="shared" si="0"/>
+        <v>9.6678857305455823E-9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>106</v>
+      </c>
+      <c r="B65" s="1">
+        <v>6.1908000000000005E-14</v>
+      </c>
+      <c r="C65" s="1">
+        <f t="shared" si="0"/>
+        <v>9.6842674778663509E-9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>107</v>
+      </c>
+      <c r="B66" s="1">
+        <v>6.1782499999999994E-14</v>
+      </c>
+      <c r="C66" s="1">
+        <f t="shared" si="0"/>
+        <v>9.7039393197062307E-9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" s="1">
+        <v>6.1801499999999994E-14</v>
+      </c>
+      <c r="C67" s="1">
+        <f t="shared" ref="C67:C92" si="1">1/((2*PI()*$B$1)^2*B67)</f>
+        <v>9.7009559803524218E-9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" s="1">
+        <v>6.1759100000000004E-14</v>
+      </c>
+      <c r="C68" s="1">
+        <f t="shared" si="1"/>
+        <v>9.7076160601393177E-9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>110</v>
+      </c>
+      <c r="B69" s="1">
+        <v>6.17362E-14</v>
+      </c>
+      <c r="C69" s="1">
+        <f t="shared" si="1"/>
+        <v>9.7112169362505333E-9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" s="1">
+        <v>6.1722100000000002E-14</v>
+      </c>
+      <c r="C70" s="1">
+        <f t="shared" si="1"/>
+        <v>9.7134353986619068E-9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>112</v>
+      </c>
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>113</v>
+      </c>
+      <c r="B73" s="1">
+        <v>4.27261E-14</v>
+      </c>
+      <c r="C73" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4032023307059388E-8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>114</v>
+      </c>
+      <c r="B74" s="1">
+        <v>4.5899899999999998E-14</v>
+      </c>
+      <c r="C74" s="1">
+        <f t="shared" si="1"/>
+        <v>1.3061763337605315E-8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>115</v>
+      </c>
+      <c r="B75" s="1">
+        <v>4.9079999999999998E-14</v>
+      </c>
+      <c r="C75" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2215436654844137E-8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>116</v>
+      </c>
+      <c r="B76" s="1">
+        <v>5.2262500000000001E-14</v>
+      </c>
+      <c r="C76" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1471583468447741E-8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>117</v>
+      </c>
+      <c r="B77" s="1">
+        <v>5.54507E-14</v>
+      </c>
+      <c r="C77" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0812011949709384E-8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="1">
+        <v>5.8644799999999997E-14</v>
+      </c>
+      <c r="C78" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0223133696759989E-8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>119</v>
+      </c>
+      <c r="B79" s="1">
+        <v>6.1855399999999996E-14</v>
+      </c>
+      <c r="C79" s="1">
+        <f t="shared" si="1"/>
+        <v>9.6925026920810491E-9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>120</v>
+      </c>
+      <c r="B80" s="1">
+        <v>6.5068099999999996E-14</v>
+      </c>
+      <c r="C80" s="1">
+        <f t="shared" si="1"/>
+        <v>9.2139409483256798E-9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B81" s="1">
+        <v>6.8315699999999997E-14</v>
+      </c>
+      <c r="C81" s="1">
+        <f t="shared" si="1"/>
+        <v>8.7759275103636519E-9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>122</v>
+      </c>
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>113</v>
+      </c>
+      <c r="B84" s="1">
+        <v>4.27261E-14</v>
+      </c>
+      <c r="C84" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4032023307059388E-8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>114</v>
+      </c>
+      <c r="B85" s="1">
+        <v>4.5899899999999998E-14</v>
+      </c>
+      <c r="C85" s="1">
+        <f t="shared" si="1"/>
+        <v>1.3061763337605315E-8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>115</v>
+      </c>
+      <c r="B86" s="1">
+        <v>4.9079999999999998E-14</v>
+      </c>
+      <c r="C86" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2215436654844137E-8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>116</v>
+      </c>
+      <c r="B87" s="1">
+        <v>5.2262500000000001E-14</v>
+      </c>
+      <c r="C87" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1471583468447741E-8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>117</v>
+      </c>
+      <c r="B88" s="1">
+        <v>5.54507E-14</v>
+      </c>
+      <c r="C88" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0812011949709384E-8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>118</v>
+      </c>
+      <c r="B89" s="1">
+        <v>5.8644799999999997E-14</v>
+      </c>
+      <c r="C89" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0223133696759989E-8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>119</v>
+      </c>
+      <c r="B90" s="1">
+        <v>6.1855399999999996E-14</v>
+      </c>
+      <c r="C90" s="1">
+        <f t="shared" si="1"/>
+        <v>9.6925026920810491E-9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>120</v>
+      </c>
+      <c r="B91" s="1">
+        <v>6.5068099999999996E-14</v>
+      </c>
+      <c r="C91" s="1">
+        <f t="shared" si="1"/>
+        <v>9.2139409483256798E-9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>121</v>
+      </c>
+      <c r="B92" s="1">
+        <v>6.8315699999999997E-14</v>
+      </c>
+      <c r="C92" s="1">
+        <f t="shared" si="1"/>
+        <v>8.7759275103636519E-9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More IBM ratios, excel updated
</commit_message>
<xml_diff>
--- a/participation_ratios.xlsx
+++ b/participation_ratios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="153">
   <si>
     <t>IBM_ratio_default</t>
   </si>
@@ -433,6 +433,48 @@
   </si>
   <si>
     <t>Inductance [H]</t>
+  </si>
+  <si>
+    <t>IBM_ratio_pad_w_300</t>
+  </si>
+  <si>
+    <t>IBM_ratio_pad_w_300_openboundary</t>
+  </si>
+  <si>
+    <t>IBM_ratio_pad_w_350</t>
+  </si>
+  <si>
+    <t>IBM_ratio_pad_w_400</t>
+  </si>
+  <si>
+    <t>IBM_ratio_pad_w_450</t>
+  </si>
+  <si>
+    <t>IBM_ratio_pad_w_500</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_cornerr_5</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_cornerr_10</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_cornerr_15</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_cornerr_20</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_cornerr_25</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_cornerr_29</t>
+  </si>
+  <si>
+    <t>Pad Width</t>
+  </si>
+  <si>
+    <t>Corner Radius</t>
   </si>
 </sst>
 </file>
@@ -541,7 +583,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -554,6 +596,7 @@
     <xf numFmtId="11" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
@@ -1256,12 +1299,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O56"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="O37" sqref="O37"/>
+      <selection pane="topRight" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2558,6 +2601,587 @@
         <v>1083873</v>
       </c>
     </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59">
+        <v>14.1416</v>
+      </c>
+      <c r="C59">
+        <v>6.5128000000000004</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1.4E-8</v>
+      </c>
+      <c r="E59" s="1">
+        <v>4.27261E-14</v>
+      </c>
+      <c r="F59" s="1">
+        <v>4.7120000000000003E-5</v>
+      </c>
+      <c r="G59" s="1">
+        <v>3.5076999999999998E-4</v>
+      </c>
+      <c r="H59" s="1">
+        <v>1.0817E-4</v>
+      </c>
+      <c r="I59" s="1">
+        <f>SUM(F59:H59)</f>
+        <v>5.0606000000000002E-4</v>
+      </c>
+      <c r="J59" s="3">
+        <v>300</v>
+      </c>
+      <c r="K59">
+        <v>18</v>
+      </c>
+      <c r="L59">
+        <v>60</v>
+      </c>
+      <c r="M59">
+        <v>650</v>
+      </c>
+      <c r="N59" t="s">
+        <v>135</v>
+      </c>
+      <c r="O59">
+        <v>735711</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B60">
+        <v>14.141500000000001</v>
+      </c>
+      <c r="C60">
+        <v>6.5171999999999999</v>
+      </c>
+      <c r="D60" s="1">
+        <v>1.4E-8</v>
+      </c>
+      <c r="E60" s="1">
+        <v>4.27261E-14</v>
+      </c>
+      <c r="I60" s="1">
+        <f t="shared" ref="I60:I64" si="1">SUM(F60:H60)</f>
+        <v>0</v>
+      </c>
+      <c r="J60" s="3">
+        <v>300</v>
+      </c>
+      <c r="K60">
+        <v>18</v>
+      </c>
+      <c r="L60">
+        <v>60</v>
+      </c>
+      <c r="M60">
+        <v>650</v>
+      </c>
+      <c r="N60" t="s">
+        <v>135</v>
+      </c>
+      <c r="O60">
+        <v>830555</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B61">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C61">
+        <v>6.51</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1.22E-8</v>
+      </c>
+      <c r="E61" s="1">
+        <v>4.9079999999999998E-14</v>
+      </c>
+      <c r="F61" s="1">
+        <v>4.2855000000000002E-5</v>
+      </c>
+      <c r="G61" s="1">
+        <v>3.4443000000000001E-4</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1.0417E-4</v>
+      </c>
+      <c r="I61" s="1">
+        <f t="shared" si="1"/>
+        <v>4.9145500000000002E-4</v>
+      </c>
+      <c r="J61" s="3">
+        <v>350</v>
+      </c>
+      <c r="K61">
+        <v>18</v>
+      </c>
+      <c r="L61">
+        <v>60</v>
+      </c>
+      <c r="M61">
+        <v>650</v>
+      </c>
+      <c r="N61" t="s">
+        <v>135</v>
+      </c>
+      <c r="O61">
+        <v>832072</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B62">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C62">
+        <v>6.5095999999999998</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1.0800000000000001E-8</v>
+      </c>
+      <c r="E62" s="1">
+        <v>5.54507E-14</v>
+      </c>
+      <c r="F62" s="1">
+        <v>4.2694000000000002E-5</v>
+      </c>
+      <c r="G62" s="1">
+        <v>3.3775E-4</v>
+      </c>
+      <c r="H62" s="1">
+        <v>1.0182E-4</v>
+      </c>
+      <c r="I62" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8226400000000004E-4</v>
+      </c>
+      <c r="J62" s="3">
+        <v>400</v>
+      </c>
+      <c r="K62">
+        <v>18</v>
+      </c>
+      <c r="L62">
+        <v>60</v>
+      </c>
+      <c r="M62">
+        <v>650</v>
+      </c>
+      <c r="N62" t="s">
+        <v>135</v>
+      </c>
+      <c r="O62">
+        <v>935539</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63">
+        <v>14.1412</v>
+      </c>
+      <c r="C63">
+        <v>6.5072000000000001</v>
+      </c>
+      <c r="D63" s="1">
+        <v>9.6899999999999994E-9</v>
+      </c>
+      <c r="E63" s="1">
+        <v>6.1855399999999996E-14</v>
+      </c>
+      <c r="F63" s="1">
+        <v>4.1739000000000001E-5</v>
+      </c>
+      <c r="G63" s="1">
+        <v>3.3197000000000001E-4</v>
+      </c>
+      <c r="H63" s="1">
+        <v>1.0068000000000001E-4</v>
+      </c>
+      <c r="I63" s="1">
+        <f t="shared" si="1"/>
+        <v>4.7438900000000003E-4</v>
+      </c>
+      <c r="J63" s="3">
+        <v>450</v>
+      </c>
+      <c r="K63">
+        <v>18</v>
+      </c>
+      <c r="L63">
+        <v>60</v>
+      </c>
+      <c r="M63">
+        <v>650</v>
+      </c>
+      <c r="N63" t="s">
+        <v>135</v>
+      </c>
+      <c r="O63">
+        <v>1038493</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64">
+        <v>14.1411</v>
+      </c>
+      <c r="C64">
+        <v>6.5052000000000003</v>
+      </c>
+      <c r="D64" s="1">
+        <v>8.7799999999999999E-9</v>
+      </c>
+      <c r="E64" s="1">
+        <v>6.8315699999999997E-14</v>
+      </c>
+      <c r="F64" s="1">
+        <v>4.0368999999999999E-5</v>
+      </c>
+      <c r="G64" s="1">
+        <v>3.2810000000000001E-4</v>
+      </c>
+      <c r="H64" s="1">
+        <v>9.9210999999999996E-5</v>
+      </c>
+      <c r="I64" s="1">
+        <f t="shared" si="1"/>
+        <v>4.6767999999999999E-4</v>
+      </c>
+      <c r="J64" s="3">
+        <v>500</v>
+      </c>
+      <c r="K64">
+        <v>18</v>
+      </c>
+      <c r="L64">
+        <v>60</v>
+      </c>
+      <c r="M64">
+        <v>650</v>
+      </c>
+      <c r="N64" t="s">
+        <v>135</v>
+      </c>
+      <c r="O64">
+        <v>1146237</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="D65" s="1"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B67">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C67">
+        <v>6.5048000000000004</v>
+      </c>
+      <c r="D67" s="1">
+        <v>9.7100000000000006E-9</v>
+      </c>
+      <c r="E67" s="1">
+        <v>6.1720000000000001E-14</v>
+      </c>
+      <c r="F67" s="1">
+        <v>3.7382999999999998E-5</v>
+      </c>
+      <c r="G67" s="1">
+        <v>3.0276000000000001E-4</v>
+      </c>
+      <c r="H67" s="1">
+        <v>9.5347999999999996E-5</v>
+      </c>
+      <c r="I67" s="1">
+        <f>SUM(F67:H67)</f>
+        <v>4.3549099999999998E-4</v>
+      </c>
+      <c r="J67">
+        <v>450</v>
+      </c>
+      <c r="K67">
+        <v>18</v>
+      </c>
+      <c r="L67">
+        <v>60</v>
+      </c>
+      <c r="M67">
+        <v>650</v>
+      </c>
+      <c r="N67" s="3">
+        <v>5</v>
+      </c>
+      <c r="O67">
+        <v>835079</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B68">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C68">
+        <v>6.5044000000000004</v>
+      </c>
+      <c r="D68" s="1">
+        <v>9.7499999999999996E-9</v>
+      </c>
+      <c r="E68" s="1">
+        <v>6.1463999999999997E-14</v>
+      </c>
+      <c r="F68" s="1">
+        <v>3.557E-5</v>
+      </c>
+      <c r="G68" s="1">
+        <v>3.0078E-4</v>
+      </c>
+      <c r="H68" s="1">
+        <v>9.4667999999999996E-5</v>
+      </c>
+      <c r="I68" s="1">
+        <f t="shared" ref="I68:I72" si="2">SUM(F68:H68)</f>
+        <v>4.3101800000000003E-4</v>
+      </c>
+      <c r="J68">
+        <v>450</v>
+      </c>
+      <c r="K68">
+        <v>18</v>
+      </c>
+      <c r="L68">
+        <v>60</v>
+      </c>
+      <c r="M68">
+        <v>650</v>
+      </c>
+      <c r="N68" s="3">
+        <v>10</v>
+      </c>
+      <c r="O68">
+        <v>831573</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C69">
+        <v>6.5027999999999997</v>
+      </c>
+      <c r="D69" s="1">
+        <v>9.8099999999999998E-9</v>
+      </c>
+      <c r="E69" s="1">
+        <v>6.1125899999999994E-14</v>
+      </c>
+      <c r="F69" s="1">
+        <v>3.6656000000000003E-5</v>
+      </c>
+      <c r="G69" s="1">
+        <v>2.9846000000000001E-4</v>
+      </c>
+      <c r="H69" s="1">
+        <v>9.6022999999999999E-5</v>
+      </c>
+      <c r="I69" s="1">
+        <f t="shared" si="2"/>
+        <v>4.3113899999999998E-4</v>
+      </c>
+      <c r="J69">
+        <v>450</v>
+      </c>
+      <c r="K69">
+        <v>18</v>
+      </c>
+      <c r="L69">
+        <v>60</v>
+      </c>
+      <c r="M69">
+        <v>650</v>
+      </c>
+      <c r="N69" s="3">
+        <v>15</v>
+      </c>
+      <c r="O69">
+        <v>824442</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B70">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C70">
+        <v>6.5019999999999998</v>
+      </c>
+      <c r="D70" s="1">
+        <v>9.8799999999999998E-9</v>
+      </c>
+      <c r="E70" s="1">
+        <v>6.0706000000000002E-14</v>
+      </c>
+      <c r="F70" s="1">
+        <v>3.3695000000000002E-5</v>
+      </c>
+      <c r="G70" s="1">
+        <v>2.9975999999999999E-4</v>
+      </c>
+      <c r="H70" s="1">
+        <v>9.5086000000000004E-5</v>
+      </c>
+      <c r="I70" s="1">
+        <f t="shared" si="2"/>
+        <v>4.2854099999999995E-4</v>
+      </c>
+      <c r="J70">
+        <v>450</v>
+      </c>
+      <c r="K70">
+        <v>18</v>
+      </c>
+      <c r="L70">
+        <v>60</v>
+      </c>
+      <c r="M70">
+        <v>650</v>
+      </c>
+      <c r="N70" s="3">
+        <v>20</v>
+      </c>
+      <c r="O70">
+        <v>817046</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C71">
+        <v>6.5255999999999998</v>
+      </c>
+      <c r="D71" s="1">
+        <v>9.9599999999999995E-9</v>
+      </c>
+      <c r="E71" s="1">
+        <v>6.0221000000000004E-14</v>
+      </c>
+      <c r="F71" s="1">
+        <v>3.4653000000000002E-5</v>
+      </c>
+      <c r="G71" s="1">
+        <v>2.9682999999999999E-4</v>
+      </c>
+      <c r="H71" s="1">
+        <v>9.4098999999999995E-5</v>
+      </c>
+      <c r="I71" s="1">
+        <f t="shared" si="2"/>
+        <v>4.2558199999999998E-4</v>
+      </c>
+      <c r="J71">
+        <v>450</v>
+      </c>
+      <c r="K71">
+        <v>18</v>
+      </c>
+      <c r="L71">
+        <v>60</v>
+      </c>
+      <c r="M71">
+        <v>650</v>
+      </c>
+      <c r="N71" s="3">
+        <v>25</v>
+      </c>
+      <c r="O71">
+        <v>799697</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C72">
+        <v>6.5124000000000004</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="E72" s="1">
+        <v>5.9773400000000001E-14</v>
+      </c>
+      <c r="F72" s="1">
+        <v>3.4888000000000002E-5</v>
+      </c>
+      <c r="G72" s="1">
+        <v>2.9881999999999999E-4</v>
+      </c>
+      <c r="H72" s="1">
+        <v>9.4730999999999998E-5</v>
+      </c>
+      <c r="I72" s="1">
+        <f t="shared" si="2"/>
+        <v>4.2843899999999997E-4</v>
+      </c>
+      <c r="J72">
+        <v>450</v>
+      </c>
+      <c r="K72">
+        <v>18</v>
+      </c>
+      <c r="L72">
+        <v>60</v>
+      </c>
+      <c r="M72">
+        <v>650</v>
+      </c>
+      <c r="N72" s="3">
+        <v>29</v>
+      </c>
+      <c r="O72">
+        <v>799697</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2568,8 +3192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,7 +4089,7 @@
         <v>4.27261E-14</v>
       </c>
       <c r="C84" s="1">
-        <f t="shared" si="1"/>
+        <f>1/((2*PI()*$B$1)^2*B84)</f>
         <v>1.4032023307059388E-8</v>
       </c>
     </row>
@@ -3567,5 +4191,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated result and discussion
</commit_message>
<xml_diff>
--- a/participation_ratios.xlsx
+++ b/participation_ratios.xlsx
@@ -921,7 +921,9 @@
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="11" max="11" width="29.42578125" customWidth="1"/>
     <col min="12" max="12" width="45.85546875" customWidth="1"/>
-    <col min="13" max="14" width="19.7109375" customWidth="1"/>
+    <col min="13" max="13" width="39.140625" customWidth="1"/>
+    <col min="14" max="14" width="39.28515625" customWidth="1"/>
+    <col min="15" max="15" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -1302,9 +1304,9 @@
   <dimension ref="A1:O72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="D37" sqref="D37"/>
+      <selection pane="topRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2671,7 +2673,7 @@
         <v>4.27261E-14</v>
       </c>
       <c r="I60" s="1">
-        <f t="shared" ref="I60:I64" si="1">SUM(F60:H60)</f>
+        <f>SUM(F60:H60)</f>
         <v>0</v>
       </c>
       <c r="J60" s="3">
@@ -2719,7 +2721,7 @@
         <v>1.0417E-4</v>
       </c>
       <c r="I61" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I60:I64" si="1">SUM(F61:H61)</f>
         <v>4.9145500000000002E-4</v>
       </c>
       <c r="J61" s="3">

</xml_diff>

<commit_message>
more new raw data
</commit_message>
<xml_diff>
--- a/participation_ratios.xlsx
+++ b/participation_ratios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855"/>
   </bookViews>
   <sheets>
     <sheet name="Ratios" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="176">
   <si>
     <t>IBM_ratio_default</t>
   </si>
@@ -534,6 +534,75 @@
       </rPr>
       <t>sep_sweep10_40</t>
     </r>
+  </si>
+  <si>
+    <t>Slot size</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_s18_slotsize_500</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_s18_slotsize_566</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_s18_slotsize_533</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_s18_slotsize_600</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_s18_slotsize_700</t>
+  </si>
+  <si>
+    <t>IBM_ratio_w450_l60_s18_slotsize_800</t>
+  </si>
+  <si>
+    <t>Pad Separation 60 fF</t>
+  </si>
+  <si>
+    <t>IBM_ratio_sep_5_l60_60fF</t>
+  </si>
+  <si>
+    <t>IBM_ratio_sep_10_l60_60fF</t>
+  </si>
+  <si>
+    <t>IBM_ratio_sep_20_l60_60fF</t>
+  </si>
+  <si>
+    <t>IBM_ratio_sep_50_l60_60fF</t>
+  </si>
+  <si>
+    <t>Yale_ratio_5fingers_rounded_r1_g_20um_l56_longer</t>
+  </si>
+  <si>
+    <t>Yale_ratio_5fingers_rounded_r8_g_20um_l56_longer</t>
+  </si>
+  <si>
+    <t>Yale_ratio_5fingers_rounded_g_20um_l56_longer</t>
+  </si>
+  <si>
+    <t>Yale_ratio_10_fingers_rounded_g_5um_l36_longer</t>
+  </si>
+  <si>
+    <t>Yale_ratio_5fingers_rounded_g_10um_l76_longer</t>
+  </si>
+  <si>
+    <t>Yale_capacitance_rounded_fingers_4</t>
+  </si>
+  <si>
+    <t>Yale_capacitance_rounded_fingers_5</t>
+  </si>
+  <si>
+    <t>Yale_capacitance_rounded_fingers_6</t>
+  </si>
+  <si>
+    <t>Yale_capacitance_rounded_fingers_7</t>
+  </si>
+  <si>
+    <t>Yale_capacitance_rounded_fingers_8</t>
+  </si>
+  <si>
+    <t>Yale_capacitance_rounded_fingers_9</t>
   </si>
 </sst>
 </file>
@@ -678,7 +747,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -784,11 +853,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70081536"/>
-        <c:axId val="70095616"/>
+        <c:axId val="65407232"/>
+        <c:axId val="65413120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70081536"/>
+        <c:axId val="65407232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -797,7 +866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70095616"/>
+        <c:crossAx val="65413120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -805,7 +874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70095616"/>
+        <c:axId val="65413120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -816,7 +885,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70081536"/>
+        <c:crossAx val="65407232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -841,7 +910,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -947,11 +1016,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70372352"/>
-        <c:axId val="70374144"/>
+        <c:axId val="65441152"/>
+        <c:axId val="65451136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70372352"/>
+        <c:axId val="65441152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -960,7 +1029,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70374144"/>
+        <c:crossAx val="65451136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -968,7 +1037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70374144"/>
+        <c:axId val="65451136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,7 +1048,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70372352"/>
+        <c:crossAx val="65441152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1004,7 +1073,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1116,11 +1185,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101340672"/>
-        <c:axId val="101342208"/>
+        <c:axId val="65741568"/>
+        <c:axId val="65743104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101340672"/>
+        <c:axId val="65741568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,7 +1198,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101342208"/>
+        <c:crossAx val="65743104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1137,7 +1206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101342208"/>
+        <c:axId val="65743104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,7 +1217,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101340672"/>
+        <c:crossAx val="65741568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1173,7 +1242,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1297,11 +1366,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70778880"/>
-        <c:axId val="101170560"/>
+        <c:axId val="65767296"/>
+        <c:axId val="65768832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70778880"/>
+        <c:axId val="65767296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1310,7 +1379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101170560"/>
+        <c:crossAx val="65768832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1318,7 +1387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101170560"/>
+        <c:axId val="65768832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1329,7 +1398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70778880"/>
+        <c:crossAx val="65767296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1354,7 +1423,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1466,11 +1535,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="71042176"/>
-        <c:axId val="71239168"/>
+        <c:axId val="65793024"/>
+        <c:axId val="68621056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71042176"/>
+        <c:axId val="65793024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,7 +1548,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71239168"/>
+        <c:crossAx val="68621056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1487,7 +1556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71239168"/>
+        <c:axId val="68621056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1498,7 +1567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71042176"/>
+        <c:crossAx val="65793024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1523,7 +1592,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1635,11 +1704,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108441600"/>
-        <c:axId val="108443136"/>
+        <c:axId val="68641536"/>
+        <c:axId val="68643072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108441600"/>
+        <c:axId val="68641536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,7 +1717,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108443136"/>
+        <c:crossAx val="68643072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1656,7 +1725,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108443136"/>
+        <c:axId val="68643072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1667,7 +1736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108441600"/>
+        <c:crossAx val="68641536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1692,7 +1761,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1780,11 +1849,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101163776"/>
-        <c:axId val="101180160"/>
+        <c:axId val="68659072"/>
+        <c:axId val="68660608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101163776"/>
+        <c:axId val="68659072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1793,7 +1862,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101180160"/>
+        <c:crossAx val="68660608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1801,7 +1870,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101180160"/>
+        <c:axId val="68660608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1812,7 +1881,126 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101163776"/>
+        <c:crossAx val="68659072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Capacitances!$B$96:$B$101</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.7172999999999999E-14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8637900000000003E-14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0343899999999998E-14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2385100000000002E-14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.466854E-14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0740223E-13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="78858496"/>
+        <c:axId val="78889728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="78858496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78889728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="78889728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78858496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2041,6 +2229,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>895349</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2338,7 +2556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2734,12 +2952,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O72"/>
+  <dimension ref="A1:O92"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="F54" sqref="F54"/>
+      <selection pane="topRight" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3018,61 +3236,38 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>169</v>
       </c>
       <c r="B24">
-        <v>14.14</v>
+        <v>14.141299999999999</v>
       </c>
       <c r="C24">
-        <v>6.5309999999999997</v>
+        <v>6.5648</v>
       </c>
       <c r="D24" s="1">
         <v>1E-8</v>
       </c>
-      <c r="E24" s="1">
-        <v>5.9999999999999997E-14</v>
-      </c>
-      <c r="F24" s="7">
-        <v>5.0957E-5</v>
-      </c>
-      <c r="G24" s="7">
-        <v>5.1272999999999998E-4</v>
-      </c>
-      <c r="H24" s="7">
-        <v>1.6066E-4</v>
-      </c>
-      <c r="I24" s="7">
-        <f>SUM(F24:H24)</f>
-        <v>7.2434699999999997E-4</v>
-      </c>
-      <c r="J24" s="2">
-        <v>5</v>
-      </c>
-      <c r="K24" s="4">
-        <v>20</v>
-      </c>
-      <c r="L24" s="4">
-        <v>56</v>
-      </c>
-      <c r="M24">
-        <v>20</v>
-      </c>
-      <c r="N24">
-        <v>10</v>
-      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
       <c r="O24">
-        <v>688893</v>
+        <v>1179186</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B25">
-        <v>14.141400000000001</v>
+        <v>14.14</v>
       </c>
       <c r="C25">
-        <v>6.6116000000000001</v>
+        <v>6.5309999999999997</v>
       </c>
       <c r="D25" s="1">
         <v>1E-8</v>
@@ -3080,261 +3275,228 @@
       <c r="E25" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="F25" s="1">
-        <v>1.3553999999999999E-4</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="H25" s="1">
-        <v>4.1235000000000002E-4</v>
-      </c>
-      <c r="I25" s="1">
+      <c r="F25" s="7">
+        <v>5.0957E-5</v>
+      </c>
+      <c r="G25" s="7">
+        <v>5.1272999999999998E-4</v>
+      </c>
+      <c r="H25" s="7">
+        <v>1.6066E-4</v>
+      </c>
+      <c r="I25" s="7">
         <f>SUM(F25:H25)</f>
-        <v>1.84789E-3</v>
+        <v>7.2434699999999997E-4</v>
       </c>
       <c r="J25" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K25" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="L25" s="4">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="M25">
         <v>20</v>
       </c>
       <c r="N25">
-        <v>2.5</v>
+        <v>10</v>
       </c>
       <c r="O25">
-        <v>660464</v>
+        <v>688893</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>167</v>
       </c>
       <c r="B26">
-        <v>14.14</v>
+        <v>14.141400000000001</v>
       </c>
       <c r="C26">
-        <v>6.5195999999999996</v>
+        <v>6.5324999999999998</v>
       </c>
       <c r="D26" s="1">
         <v>1E-8</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="1"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="4">
+        <v>20</v>
+      </c>
+      <c r="L26" s="4">
+        <v>56</v>
+      </c>
+      <c r="O26">
+        <v>1.2019169999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C27">
+        <v>6.6116000000000001</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="E27" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F27" s="1">
+        <v>1.3553999999999999E-4</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="H27" s="1">
+        <v>4.1235000000000002E-4</v>
+      </c>
+      <c r="I27" s="1">
+        <f>SUM(F27:H27)</f>
+        <v>1.84789E-3</v>
+      </c>
+      <c r="J27" s="2">
+        <v>10</v>
+      </c>
+      <c r="K27" s="4">
+        <v>5</v>
+      </c>
+      <c r="L27" s="4">
+        <v>36</v>
+      </c>
+      <c r="M27">
+        <v>20</v>
+      </c>
+      <c r="N27">
+        <v>2.5</v>
+      </c>
+      <c r="O27">
+        <v>660464</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B28">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C28">
+        <v>6.6204000000000001</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="4">
+        <v>5</v>
+      </c>
+      <c r="L28" s="4">
+        <v>36</v>
+      </c>
+      <c r="O28">
+        <v>997800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>14.14</v>
+      </c>
+      <c r="C29">
+        <v>6.5195999999999996</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="E29" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="F29" s="1">
         <v>7.5575999999999996E-5</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G29" s="1">
         <v>7.3333000000000003E-4</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H29" s="1">
         <v>2.4617999999999998E-4</v>
       </c>
-      <c r="I26" s="1">
-        <f>SUM(F26:H26)</f>
+      <c r="I29" s="1">
+        <f>SUM(F29:H29)</f>
         <v>1.055086E-3</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J29" s="2">
         <v>10</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K29" s="4">
         <v>10</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L29" s="4">
         <v>26</v>
       </c>
-      <c r="M26">
+      <c r="M29">
         <v>20</v>
       </c>
-      <c r="N26">
+      <c r="N29">
         <v>5</v>
       </c>
-      <c r="O26">
+      <c r="O29">
         <v>1051136</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30">
-        <v>14.141400000000001</v>
-      </c>
-      <c r="C30">
-        <v>6.5044000000000004</v>
-      </c>
-      <c r="E30" s="1">
-        <v>6.3499999999999994E-14</v>
-      </c>
-      <c r="F30" s="1">
-        <v>5.7122E-5</v>
-      </c>
-      <c r="G30" s="1">
-        <v>5.3123000000000005E-4</v>
-      </c>
-      <c r="H30" s="1">
-        <v>1.784E-4</v>
-      </c>
-      <c r="I30" s="1">
-        <f>SUM(F30:H30)</f>
-        <v>7.667520000000001E-4</v>
-      </c>
-      <c r="J30" s="2">
-        <v>5</v>
-      </c>
-      <c r="K30" s="2">
-        <v>20</v>
-      </c>
-      <c r="L30" s="2">
-        <v>56</v>
-      </c>
-      <c r="M30" s="3">
-        <v>10</v>
-      </c>
-      <c r="N30" s="2">
-        <v>10</v>
-      </c>
-      <c r="O30" s="2">
-        <v>702518</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31">
-        <v>14.141299999999999</v>
-      </c>
-      <c r="C31">
-        <v>6.5035999999999996</v>
-      </c>
-      <c r="E31" s="1">
-        <v>5.9700000000000001E-14</v>
-      </c>
-      <c r="F31" s="7">
-        <v>6.1889000000000003E-5</v>
-      </c>
-      <c r="G31" s="7">
-        <v>5.4920000000000001E-4</v>
-      </c>
-      <c r="H31" s="7">
-        <v>1.7187999999999999E-4</v>
-      </c>
-      <c r="I31" s="7">
-        <f>SUM(F31:H31)</f>
-        <v>7.82969E-4</v>
-      </c>
-      <c r="J31" s="2">
-        <v>5</v>
-      </c>
-      <c r="K31" s="2">
-        <v>20</v>
-      </c>
-      <c r="L31" s="2">
-        <v>56</v>
-      </c>
-      <c r="M31" s="3">
-        <v>20</v>
-      </c>
-      <c r="N31" s="2">
-        <v>10</v>
-      </c>
-      <c r="O31" s="2">
-        <v>886630</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32">
-        <v>14.141400000000001</v>
-      </c>
-      <c r="C32">
-        <v>6.5044000000000004</v>
-      </c>
-      <c r="E32" s="1">
-        <v>5.6800000000000002E-14</v>
-      </c>
-      <c r="F32" s="1">
-        <v>5.2184E-5</v>
-      </c>
-      <c r="G32" s="1">
-        <v>5.0383999999999997E-4</v>
-      </c>
-      <c r="H32" s="1">
-        <v>1.6097E-4</v>
-      </c>
-      <c r="I32" s="1">
-        <f>SUM(F32:H32)</f>
-        <v>7.1699399999999999E-4</v>
-      </c>
-      <c r="J32" s="2">
-        <v>5</v>
-      </c>
-      <c r="K32" s="2">
-        <v>20</v>
-      </c>
-      <c r="L32" s="2">
-        <v>56</v>
-      </c>
-      <c r="M32" s="3">
-        <v>50</v>
-      </c>
-      <c r="N32" s="2">
-        <v>10</v>
-      </c>
-      <c r="O32" s="2">
-        <v>789245</v>
-      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B33">
         <v>14.141400000000001</v>
       </c>
       <c r="C33">
-        <v>6.5019999999999998</v>
+        <v>6.5044000000000004</v>
       </c>
       <c r="E33" s="1">
-        <v>5.58E-14</v>
+        <v>6.3499999999999994E-14</v>
       </c>
       <c r="F33" s="1">
-        <v>4.8152000000000002E-5</v>
+        <v>5.7122E-5</v>
       </c>
       <c r="G33" s="1">
-        <v>4.9222000000000003E-4</v>
+        <v>5.3123000000000005E-4</v>
       </c>
       <c r="H33" s="1">
-        <v>1.5393000000000001E-4</v>
+        <v>1.784E-4</v>
       </c>
       <c r="I33" s="1">
         <f>SUM(F33:H33)</f>
-        <v>6.9430200000000005E-4</v>
+        <v>7.667520000000001E-4</v>
       </c>
       <c r="J33" s="2">
         <v>5</v>
@@ -3346,40 +3508,40 @@
         <v>56</v>
       </c>
       <c r="M33" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="N33" s="2">
         <v>10</v>
       </c>
       <c r="O33" s="2">
-        <v>670572</v>
+        <v>702518</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B34">
-        <v>14.141500000000001</v>
+        <v>14.141299999999999</v>
       </c>
       <c r="C34">
-        <v>6.5031999999999996</v>
+        <v>6.5035999999999996</v>
       </c>
       <c r="E34" s="1">
-        <v>5.5400000000000002E-14</v>
-      </c>
-      <c r="F34" s="1">
-        <v>5.0986000000000003E-5</v>
-      </c>
-      <c r="G34" s="1">
-        <v>4.8979999999999998E-4</v>
-      </c>
-      <c r="H34" s="1">
-        <v>1.5875000000000001E-4</v>
-      </c>
-      <c r="I34" s="1">
+        <v>5.9700000000000001E-14</v>
+      </c>
+      <c r="F34" s="7">
+        <v>6.1889000000000003E-5</v>
+      </c>
+      <c r="G34" s="7">
+        <v>5.4920000000000001E-4</v>
+      </c>
+      <c r="H34" s="7">
+        <v>1.7187999999999999E-4</v>
+      </c>
+      <c r="I34" s="7">
         <f>SUM(F34:H34)</f>
-        <v>6.9953600000000006E-4</v>
+        <v>7.82969E-4</v>
       </c>
       <c r="J34" s="2">
         <v>5</v>
@@ -3391,51 +3553,130 @@
         <v>56</v>
       </c>
       <c r="M34" s="3">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="N34" s="2">
         <v>10</v>
       </c>
       <c r="O34" s="2">
-        <v>684785</v>
+        <v>886630</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C35">
+        <v>6.5044000000000004</v>
+      </c>
+      <c r="E35" s="1">
+        <v>5.6800000000000002E-14</v>
+      </c>
+      <c r="F35" s="1">
+        <v>5.2184E-5</v>
+      </c>
+      <c r="G35" s="1">
+        <v>5.0383999999999997E-4</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1.6097E-4</v>
+      </c>
+      <c r="I35" s="1">
+        <f>SUM(F35:H35)</f>
+        <v>7.1699399999999999E-4</v>
+      </c>
+      <c r="J35" s="2">
+        <v>5</v>
+      </c>
+      <c r="K35" s="2">
+        <v>20</v>
+      </c>
+      <c r="L35" s="2">
+        <v>56</v>
+      </c>
+      <c r="M35" s="3">
+        <v>50</v>
+      </c>
+      <c r="N35" s="2">
+        <v>10</v>
+      </c>
+      <c r="O35" s="2">
+        <v>789245</v>
+      </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C36">
+        <v>6.5019999999999998</v>
+      </c>
+      <c r="E36" s="1">
+        <v>5.58E-14</v>
+      </c>
+      <c r="F36" s="1">
+        <v>4.8152000000000002E-5</v>
+      </c>
+      <c r="G36" s="1">
+        <v>4.9222000000000003E-4</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1.5393000000000001E-4</v>
+      </c>
+      <c r="I36" s="1">
+        <f>SUM(F36:H36)</f>
+        <v>6.9430200000000005E-4</v>
+      </c>
+      <c r="J36" s="2">
+        <v>5</v>
+      </c>
+      <c r="K36" s="2">
+        <v>20</v>
+      </c>
+      <c r="L36" s="2">
+        <v>56</v>
+      </c>
+      <c r="M36" s="3">
+        <v>100</v>
+      </c>
+      <c r="N36" s="2">
+        <v>10</v>
+      </c>
+      <c r="O36" s="2">
+        <v>670572</v>
+      </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B37">
-        <v>14.141400000000001</v>
+        <v>14.141500000000001</v>
       </c>
       <c r="C37">
-        <v>6.5743999999999998</v>
+        <v>6.5031999999999996</v>
       </c>
       <c r="E37" s="1">
-        <v>6.1700000000000005E-14</v>
-      </c>
-      <c r="F37" s="7">
-        <v>5.1010000000000001E-5</v>
-      </c>
-      <c r="G37" s="7">
-        <v>5.3839000000000003E-4</v>
-      </c>
-      <c r="H37" s="7">
-        <v>1.7016000000000001E-4</v>
-      </c>
-      <c r="I37" s="7">
+        <v>5.5400000000000002E-14</v>
+      </c>
+      <c r="F37" s="1">
+        <v>5.0986000000000003E-5</v>
+      </c>
+      <c r="G37" s="1">
+        <v>4.8979999999999998E-4</v>
+      </c>
+      <c r="H37" s="1">
+        <v>1.5875000000000001E-4</v>
+      </c>
+      <c r="I37" s="1">
         <f>SUM(F37:H37)</f>
-        <v>7.5956000000000005E-4</v>
+        <v>6.9953600000000006E-4</v>
       </c>
       <c r="J37" s="2">
         <v>5</v>
@@ -3446,131 +3687,52 @@
       <c r="L37" s="2">
         <v>56</v>
       </c>
-      <c r="M37">
-        <v>20</v>
-      </c>
-      <c r="N37" s="3">
-        <v>1</v>
-      </c>
-      <c r="O37" s="11">
-        <v>706509</v>
+      <c r="M37" s="3">
+        <v>200</v>
+      </c>
+      <c r="N37" s="2">
+        <v>10</v>
+      </c>
+      <c r="O37" s="2">
+        <v>684785</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38">
-        <v>14.1411</v>
-      </c>
-      <c r="C38">
-        <v>6.5712000000000002</v>
-      </c>
-      <c r="E38" s="1">
-        <v>6.1700000000000005E-14</v>
-      </c>
-      <c r="F38" s="1">
-        <v>6.5668999999999998E-5</v>
-      </c>
-      <c r="G38" s="1">
-        <v>5.9962999999999998E-4</v>
-      </c>
-      <c r="H38" s="1">
-        <v>1.8195E-4</v>
-      </c>
-      <c r="I38" s="1">
-        <f>SUM(F38:H38)</f>
-        <v>8.4724900000000001E-4</v>
-      </c>
-      <c r="J38" s="2">
-        <v>5</v>
-      </c>
-      <c r="K38" s="2">
-        <v>20</v>
-      </c>
-      <c r="L38" s="2">
-        <v>56</v>
-      </c>
-      <c r="M38">
-        <v>20</v>
-      </c>
-      <c r="N38" s="3">
-        <v>2</v>
-      </c>
-      <c r="O38">
-        <v>1105979</v>
-      </c>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39">
-        <v>14.1412</v>
-      </c>
-      <c r="C39">
-        <v>6.5784000000000002</v>
-      </c>
-      <c r="E39" s="1">
-        <v>6.1500000000000003E-14</v>
-      </c>
-      <c r="F39" s="1">
-        <v>6.6193999999999997E-5</v>
-      </c>
-      <c r="G39" s="1">
-        <v>5.7569000000000001E-4</v>
-      </c>
-      <c r="H39" s="1">
-        <v>1.7843000000000001E-4</v>
-      </c>
-      <c r="I39" s="1">
-        <f>SUM(F39:H39)</f>
-        <v>8.2031400000000005E-4</v>
-      </c>
-      <c r="J39" s="2">
-        <v>5</v>
-      </c>
-      <c r="K39" s="2">
-        <v>20</v>
-      </c>
-      <c r="L39" s="2">
-        <v>56</v>
-      </c>
-      <c r="M39">
-        <v>20</v>
-      </c>
-      <c r="N39" s="3">
-        <v>5</v>
-      </c>
-      <c r="O39">
-        <v>1194951</v>
-      </c>
+      <c r="A39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40">
         <v>14.141400000000001</v>
       </c>
       <c r="C40">
-        <v>6.4984000000000002</v>
+        <v>6.5743999999999998</v>
       </c>
       <c r="E40" s="1">
-        <v>5.9700000000000001E-14</v>
-      </c>
-      <c r="F40" s="1">
-        <v>5.0727999999999999E-5</v>
-      </c>
-      <c r="G40" s="1">
-        <v>5.2514E-4</v>
-      </c>
-      <c r="H40" s="1">
-        <v>1.6347000000000001E-4</v>
-      </c>
-      <c r="I40" s="1">
+        <v>6.1700000000000005E-14</v>
+      </c>
+      <c r="F40" s="7">
+        <v>5.1010000000000001E-5</v>
+      </c>
+      <c r="G40" s="7">
+        <v>5.3839000000000003E-4</v>
+      </c>
+      <c r="H40" s="7">
+        <v>1.7016000000000001E-4</v>
+      </c>
+      <c r="I40" s="7">
         <f>SUM(F40:H40)</f>
-        <v>7.3933799999999997E-4</v>
+        <v>7.5956000000000005E-4</v>
       </c>
       <c r="J40" s="2">
         <v>5</v>
@@ -3585,583 +3747,628 @@
         <v>20</v>
       </c>
       <c r="N40" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O40" s="11">
-        <v>696744</v>
+        <v>706509</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
+      <c r="A41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B41">
+        <v>14.1412</v>
+      </c>
+      <c r="C41">
+        <v>6.5819999999999999</v>
+      </c>
+      <c r="D41" s="1">
+        <v>9.7170000000000003E-9</v>
+      </c>
+      <c r="E41" s="1"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="N41" s="3">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>1105331</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E42" s="1"/>
-      <c r="J42" s="2"/>
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <v>14.1411</v>
+      </c>
+      <c r="C42">
+        <v>6.5712000000000002</v>
+      </c>
+      <c r="E42" s="1">
+        <v>6.1700000000000005E-14</v>
+      </c>
+      <c r="F42" s="1">
+        <v>6.5668999999999998E-5</v>
+      </c>
+      <c r="G42" s="1">
+        <v>5.9962999999999998E-4</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1.8195E-4</v>
+      </c>
+      <c r="I42" s="1">
+        <f>SUM(F42:H42)</f>
+        <v>8.4724900000000001E-4</v>
+      </c>
+      <c r="J42" s="2">
+        <v>5</v>
+      </c>
+      <c r="K42" s="2">
+        <v>20</v>
+      </c>
+      <c r="L42" s="2">
+        <v>56</v>
+      </c>
+      <c r="M42">
+        <v>20</v>
+      </c>
+      <c r="N42" s="3">
+        <v>2</v>
+      </c>
+      <c r="O42">
+        <v>1105979</v>
+      </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B43">
-        <v>14.14</v>
+        <v>14.1412</v>
       </c>
       <c r="C43">
-        <v>6.5380000000000003</v>
+        <v>6.5784000000000002</v>
       </c>
       <c r="E43" s="1">
-        <v>7.8800000000000002E-14</v>
+        <v>6.1500000000000003E-14</v>
       </c>
       <c r="F43" s="1">
-        <v>1.2299E-5</v>
+        <v>6.6193999999999997E-5</v>
       </c>
       <c r="G43" s="1">
-        <v>1.0498E-4</v>
+        <v>5.7569000000000001E-4</v>
       </c>
       <c r="H43" s="1">
-        <v>3.3423000000000002E-5</v>
+        <v>1.7843000000000001E-4</v>
       </c>
       <c r="I43" s="1">
         <f>SUM(F43:H43)</f>
-        <v>1.5070200000000001E-4</v>
-      </c>
-      <c r="J43" s="2"/>
+        <v>8.2031400000000005E-4</v>
+      </c>
+      <c r="J43" s="2">
+        <v>5</v>
+      </c>
+      <c r="K43" s="2">
+        <v>20</v>
+      </c>
+      <c r="L43" s="2">
+        <v>56</v>
+      </c>
+      <c r="M43">
+        <v>20</v>
+      </c>
+      <c r="N43" s="3">
+        <v>5</v>
+      </c>
       <c r="O43">
-        <v>667194</v>
+        <v>1194951</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J44" s="2"/>
+      <c r="A44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C44">
+        <v>6.4984000000000002</v>
+      </c>
+      <c r="E44" s="1">
+        <v>5.9700000000000001E-14</v>
+      </c>
+      <c r="F44" s="1">
+        <v>5.0727999999999999E-5</v>
+      </c>
+      <c r="G44" s="1">
+        <v>5.2514E-4</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1.6347000000000001E-4</v>
+      </c>
+      <c r="I44" s="1">
+        <f>SUM(F44:H44)</f>
+        <v>7.3933799999999997E-4</v>
+      </c>
+      <c r="J44" s="2">
+        <v>5</v>
+      </c>
+      <c r="K44" s="2">
+        <v>20</v>
+      </c>
+      <c r="L44" s="2">
+        <v>56</v>
+      </c>
+      <c r="M44">
+        <v>20</v>
+      </c>
+      <c r="N44" s="3">
+        <v>8</v>
+      </c>
+      <c r="O44" s="11">
+        <v>696744</v>
+      </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>166</v>
+      </c>
+      <c r="B45">
+        <v>14.1412</v>
+      </c>
+      <c r="C45">
+        <v>6.5060000000000002</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1.0039999999999999E-8</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="N45" s="3"/>
+      <c r="O45">
+        <v>1089415</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="N46" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E47" s="1"/>
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48">
+        <v>14.14</v>
+      </c>
+      <c r="C48">
+        <v>6.5380000000000003</v>
+      </c>
+      <c r="E48" s="1">
+        <v>7.8800000000000002E-14</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1.2299E-5</v>
+      </c>
+      <c r="G48" s="1">
+        <v>1.0498E-4</v>
+      </c>
+      <c r="H48" s="1">
+        <v>3.3423000000000002E-5</v>
+      </c>
+      <c r="I48" s="1">
+        <f>SUM(F48:H48)</f>
+        <v>1.5070200000000001E-4</v>
+      </c>
+      <c r="J48" s="2"/>
+      <c r="O48">
+        <v>667194</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>23</v>
       </c>
-      <c r="B45">
+      <c r="B50">
         <v>14.14</v>
       </c>
-      <c r="C45">
+      <c r="C50">
         <v>6.55</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E50" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F50" s="1">
         <v>1.8599999999999999E-4</v>
       </c>
-      <c r="G45" s="1">
+      <c r="G50" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H50" s="1">
         <v>4.9399999999999997E-4</v>
       </c>
-      <c r="I45" s="1">
-        <f>SUM(F45:H45)</f>
+      <c r="I50" s="1">
+        <f>SUM(F50:H50)</f>
         <v>2.2799999999999999E-3</v>
       </c>
-      <c r="J45" s="2">
+      <c r="J50" s="2">
         <v>5</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K50" s="2">
         <v>5</v>
       </c>
-      <c r="L45" s="2">
+      <c r="L50" s="2">
         <v>86.9</v>
       </c>
-      <c r="M45" s="2">
+      <c r="M50" s="2">
         <v>20</v>
       </c>
-      <c r="N45" s="2">
+      <c r="N50" s="2">
         <v>2.5</v>
       </c>
-      <c r="O45" s="2">
+      <c r="O50" s="2">
         <v>1247728</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>24</v>
       </c>
-      <c r="B46">
+      <c r="B51">
         <v>14.14</v>
       </c>
-      <c r="C46">
+      <c r="C51">
         <v>6.4939999999999998</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E51" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F51" s="1">
         <v>1.0895000000000001E-4</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G51" s="1">
         <v>9.7369999999999998E-4</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H51" s="1">
         <v>2.9263999999999999E-4</v>
       </c>
-      <c r="I46" s="1">
-        <f>SUM(F46:H46)</f>
+      <c r="I51" s="1">
+        <f>SUM(F51:H51)</f>
         <v>1.3752899999999999E-3</v>
       </c>
-      <c r="J46" s="2">
+      <c r="J51" s="2">
         <v>5</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K51" s="2">
         <v>10</v>
       </c>
-      <c r="L46" s="2">
+      <c r="L51" s="2">
         <v>78.400000000000006</v>
       </c>
-      <c r="M46" s="2">
+      <c r="M51" s="2">
         <v>20</v>
       </c>
-      <c r="N46" s="2">
+      <c r="N51" s="2">
         <v>5</v>
       </c>
-      <c r="O46" s="2">
+      <c r="O51" s="2">
         <v>1513610</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>22</v>
       </c>
-      <c r="B47">
+      <c r="B52">
         <v>14.14</v>
       </c>
-      <c r="C47" s="11">
+      <c r="C52" s="11">
         <v>6.6580000000000004</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E52" s="1">
         <v>5.9999999999999997E-14</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F52" s="1">
         <v>7.0760999999999996E-5</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G52" s="1">
         <v>5.6015000000000004E-4</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H52" s="1">
         <v>1.8159E-4</v>
       </c>
-      <c r="I47" s="1">
-        <f>SUM(F47:H47)</f>
+      <c r="I52" s="1">
+        <f>SUM(F52:H52)</f>
         <v>8.1250100000000009E-4</v>
       </c>
-      <c r="J47" s="2">
+      <c r="J52" s="2">
         <v>5</v>
       </c>
-      <c r="K47" s="2">
+      <c r="K52" s="2">
         <v>20</v>
       </c>
-      <c r="L47" s="2">
+      <c r="L52" s="2">
         <v>56.9</v>
       </c>
-      <c r="M47" s="2">
+      <c r="M52" s="2">
         <v>20</v>
       </c>
-      <c r="N47" s="2">
+      <c r="N52" s="2">
         <v>10</v>
       </c>
-      <c r="O47" s="2">
+      <c r="O52" s="2">
         <v>1373883</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="2"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
+    <row r="55" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B55" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C55" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6" t="s">
+      <c r="D55" s="6"/>
+      <c r="E55" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="F55" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G50" s="6" t="s">
+      <c r="G55" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H50" s="6" t="s">
+      <c r="H55" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I50" s="6" t="s">
+      <c r="I55" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="J50" s="6" t="s">
+      <c r="J55" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="K50" s="6" t="s">
+      <c r="K55" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="L50" s="6" t="s">
+      <c r="L55" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="M50" s="6" t="s">
+      <c r="M55" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="N50" s="6" t="s">
+      <c r="N55" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="O50" s="6" t="s">
+      <c r="O55" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J51" s="3" t="s">
+      <c r="J56" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K51" s="3"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+      <c r="K56" s="3"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B58" s="1">
         <v>14.141</v>
       </c>
-      <c r="C53">
+      <c r="C58">
         <v>6.5072000000000001</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E58" s="1">
         <v>8.0647E-14</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F58" s="1">
         <v>6.4206000000000002E-5</v>
       </c>
-      <c r="G53" s="1">
+      <c r="G58" s="1">
         <v>5.9539E-4</v>
       </c>
-      <c r="H53" s="1">
+      <c r="H58" s="1">
         <v>1.8191999999999999E-4</v>
       </c>
-      <c r="I53" s="1">
-        <f>SUM(F53:H53)</f>
+      <c r="I58" s="1">
+        <f>SUM(F58:H58)</f>
         <v>8.4151600000000005E-4</v>
       </c>
-      <c r="J53">
+      <c r="J58">
         <v>450</v>
       </c>
-      <c r="K53" s="3">
+      <c r="K58" s="3">
         <v>5</v>
       </c>
-      <c r="L53">
+      <c r="L58">
         <v>60</v>
       </c>
-      <c r="M53">
+      <c r="M58">
         <v>650</v>
       </c>
-      <c r="N53" t="s">
+      <c r="N58" t="s">
         <v>132</v>
       </c>
-      <c r="O53">
+      <c r="O58">
         <v>934556</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B59" s="1">
         <v>14.1411</v>
       </c>
-      <c r="C54">
+      <c r="C59">
         <v>6.5056000000000003</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E59" s="1">
         <v>7.0170000000000005E-14</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F59" s="1">
         <v>4.6547E-5</v>
       </c>
-      <c r="G54" s="1">
+      <c r="G59" s="1">
         <v>4.2583999999999998E-4</v>
       </c>
-      <c r="H54" s="1">
+      <c r="H59" s="1">
         <v>1.2769999999999999E-4</v>
       </c>
-      <c r="I54" s="1">
-        <f t="shared" ref="I54:I56" si="0">SUM(F54:H54)</f>
+      <c r="I59" s="1">
+        <f t="shared" ref="I59:I61" si="0">SUM(F59:H59)</f>
         <v>6.0008700000000002E-4</v>
       </c>
-      <c r="J54">
+      <c r="J59">
         <v>450</v>
       </c>
-      <c r="K54" s="3">
+      <c r="K59" s="3">
         <v>10</v>
       </c>
-      <c r="L54">
+      <c r="L59">
         <v>60</v>
       </c>
-      <c r="M54">
+      <c r="M59">
         <v>650</v>
       </c>
-      <c r="N54" t="s">
+      <c r="N59" t="s">
         <v>132</v>
       </c>
-      <c r="O54">
+      <c r="O59">
         <v>995525</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B55">
+      <c r="B60">
         <v>14.141299999999999</v>
       </c>
-      <c r="C55">
+      <c r="C60">
         <v>6.5044000000000004</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E60" s="1">
         <v>6.0391000000000005E-14</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F60" s="1">
         <v>4.0198999999999999E-5</v>
       </c>
-      <c r="G55" s="1">
+      <c r="G60" s="1">
         <v>3.2086000000000001E-4</v>
       </c>
-      <c r="H55" s="1">
+      <c r="H60" s="1">
         <v>9.6681000000000005E-5</v>
       </c>
-      <c r="I55" s="1">
+      <c r="I60" s="1">
         <f t="shared" si="0"/>
         <v>4.5773999999999999E-4</v>
       </c>
-      <c r="J55">
+      <c r="J60">
         <v>450</v>
       </c>
-      <c r="K55" s="3">
+      <c r="K60" s="3">
         <v>20</v>
       </c>
-      <c r="L55">
+      <c r="L60">
         <v>60</v>
       </c>
-      <c r="M55">
+      <c r="M60">
         <v>650</v>
       </c>
-      <c r="N55" t="s">
+      <c r="N60" t="s">
         <v>132</v>
       </c>
-      <c r="O55">
+      <c r="O60">
         <v>1041000</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B56">
+      <c r="B61">
         <v>14.141400000000001</v>
       </c>
-      <c r="C56">
+      <c r="C61">
         <v>6.5060000000000002</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E61" s="1">
         <v>4.9340000000000001E-14</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F61" s="1">
         <v>3.3513999999999998E-5</v>
       </c>
-      <c r="G56" s="1">
+      <c r="G61" s="1">
         <v>2.5494E-4</v>
       </c>
-      <c r="H56" s="1">
+      <c r="H61" s="1">
         <v>7.6984999999999996E-5</v>
       </c>
-      <c r="I56" s="1">
+      <c r="I61" s="1">
         <f t="shared" si="0"/>
         <v>3.6543900000000001E-4</v>
       </c>
-      <c r="J56">
+      <c r="J61">
         <v>450</v>
       </c>
-      <c r="K56" s="3">
+      <c r="K61" s="3">
         <v>50</v>
-      </c>
-      <c r="L56">
-        <v>60</v>
-      </c>
-      <c r="M56">
-        <v>650</v>
-      </c>
-      <c r="N56" t="s">
-        <v>132</v>
-      </c>
-      <c r="O56">
-        <v>1083873</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B59">
-        <v>14.1416</v>
-      </c>
-      <c r="C59">
-        <v>6.5128000000000004</v>
-      </c>
-      <c r="D59" s="1">
-        <v>1.4E-8</v>
-      </c>
-      <c r="E59" s="1">
-        <v>4.27261E-14</v>
-      </c>
-      <c r="F59" s="1">
-        <v>4.7120000000000003E-5</v>
-      </c>
-      <c r="G59" s="1">
-        <v>3.5076999999999998E-4</v>
-      </c>
-      <c r="H59" s="1">
-        <v>1.0817E-4</v>
-      </c>
-      <c r="I59" s="1">
-        <f>SUM(F59:H59)</f>
-        <v>5.0606000000000002E-4</v>
-      </c>
-      <c r="J59" s="3">
-        <v>300</v>
-      </c>
-      <c r="K59">
-        <v>18</v>
-      </c>
-      <c r="L59">
-        <v>60</v>
-      </c>
-      <c r="M59">
-        <v>650</v>
-      </c>
-      <c r="N59" t="s">
-        <v>132</v>
-      </c>
-      <c r="O59">
-        <v>735711</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B60">
-        <v>14.141500000000001</v>
-      </c>
-      <c r="C60">
-        <v>6.5171999999999999</v>
-      </c>
-      <c r="D60" s="1">
-        <v>1.4E-8</v>
-      </c>
-      <c r="E60" s="1">
-        <v>4.27261E-14</v>
-      </c>
-      <c r="I60" s="1">
-        <f>SUM(F60:H60)</f>
-        <v>0</v>
-      </c>
-      <c r="J60" s="3">
-        <v>300</v>
-      </c>
-      <c r="K60">
-        <v>18</v>
-      </c>
-      <c r="L60">
-        <v>60</v>
-      </c>
-      <c r="M60">
-        <v>650</v>
-      </c>
-      <c r="N60" t="s">
-        <v>132</v>
-      </c>
-      <c r="O60">
-        <v>830555</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B61">
-        <v>14.141400000000001</v>
-      </c>
-      <c r="C61">
-        <v>6.51</v>
-      </c>
-      <c r="D61" s="1">
-        <v>1.22E-8</v>
-      </c>
-      <c r="E61" s="1">
-        <v>4.9079999999999998E-14</v>
-      </c>
-      <c r="F61" s="1">
-        <v>4.2855000000000002E-5</v>
-      </c>
-      <c r="G61" s="1">
-        <v>3.4443000000000001E-4</v>
-      </c>
-      <c r="H61" s="1">
-        <v>1.0417E-4</v>
-      </c>
-      <c r="I61" s="1">
-        <f t="shared" ref="I61:I64" si="1">SUM(F61:H61)</f>
-        <v>4.9145500000000002E-4</v>
-      </c>
-      <c r="J61" s="3">
-        <v>350</v>
-      </c>
-      <c r="K61">
-        <v>18</v>
       </c>
       <c r="L61">
         <v>60</v>
@@ -4173,449 +4380,850 @@
         <v>132</v>
       </c>
       <c r="O61">
+        <v>1083873</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B64">
+        <v>14.1416</v>
+      </c>
+      <c r="C64">
+        <v>6.5128000000000004</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1.4E-8</v>
+      </c>
+      <c r="E64" s="1">
+        <v>4.27261E-14</v>
+      </c>
+      <c r="F64" s="1">
+        <v>4.7120000000000003E-5</v>
+      </c>
+      <c r="G64" s="1">
+        <v>3.5076999999999998E-4</v>
+      </c>
+      <c r="H64" s="1">
+        <v>1.0817E-4</v>
+      </c>
+      <c r="I64" s="1">
+        <f>SUM(F64:H64)</f>
+        <v>5.0606000000000002E-4</v>
+      </c>
+      <c r="J64" s="3">
+        <v>300</v>
+      </c>
+      <c r="K64">
+        <v>18</v>
+      </c>
+      <c r="L64">
+        <v>60</v>
+      </c>
+      <c r="M64">
+        <v>650</v>
+      </c>
+      <c r="N64" t="s">
+        <v>132</v>
+      </c>
+      <c r="O64">
+        <v>735711</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B65">
+        <v>14.141500000000001</v>
+      </c>
+      <c r="C65">
+        <v>6.5171999999999999</v>
+      </c>
+      <c r="D65" s="1">
+        <v>1.4E-8</v>
+      </c>
+      <c r="E65" s="1">
+        <v>4.27261E-14</v>
+      </c>
+      <c r="I65" s="1">
+        <f>SUM(F65:H65)</f>
+        <v>0</v>
+      </c>
+      <c r="J65" s="3">
+        <v>300</v>
+      </c>
+      <c r="K65">
+        <v>18</v>
+      </c>
+      <c r="L65">
+        <v>60</v>
+      </c>
+      <c r="M65">
+        <v>650</v>
+      </c>
+      <c r="N65" t="s">
+        <v>132</v>
+      </c>
+      <c r="O65">
+        <v>830555</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B66">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C66">
+        <v>6.51</v>
+      </c>
+      <c r="D66" s="1">
+        <v>1.22E-8</v>
+      </c>
+      <c r="E66" s="1">
+        <v>4.9079999999999998E-14</v>
+      </c>
+      <c r="F66" s="1">
+        <v>4.2855000000000002E-5</v>
+      </c>
+      <c r="G66" s="1">
+        <v>3.4443000000000001E-4</v>
+      </c>
+      <c r="H66" s="1">
+        <v>1.0417E-4</v>
+      </c>
+      <c r="I66" s="1">
+        <f t="shared" ref="I66:I69" si="1">SUM(F66:H66)</f>
+        <v>4.9145500000000002E-4</v>
+      </c>
+      <c r="J66" s="3">
+        <v>350</v>
+      </c>
+      <c r="K66">
+        <v>18</v>
+      </c>
+      <c r="L66">
+        <v>60</v>
+      </c>
+      <c r="M66">
+        <v>650</v>
+      </c>
+      <c r="N66" t="s">
+        <v>132</v>
+      </c>
+      <c r="O66">
         <v>832072</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B62">
+      <c r="B67">
         <v>14.141299999999999</v>
       </c>
-      <c r="C62">
+      <c r="C67">
         <v>6.5095999999999998</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D67" s="1">
         <v>1.0800000000000001E-8</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E67" s="1">
         <v>5.54507E-14</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F67" s="1">
         <v>4.2694000000000002E-5</v>
       </c>
-      <c r="G62" s="1">
+      <c r="G67" s="1">
         <v>3.3775E-4</v>
       </c>
-      <c r="H62" s="1">
+      <c r="H67" s="1">
         <v>1.0182E-4</v>
       </c>
-      <c r="I62" s="1">
+      <c r="I67" s="1">
         <f t="shared" si="1"/>
         <v>4.8226400000000004E-4</v>
       </c>
-      <c r="J62" s="3">
+      <c r="J67" s="3">
         <v>400</v>
       </c>
-      <c r="K62">
+      <c r="K67">
         <v>18</v>
       </c>
-      <c r="L62">
+      <c r="L67">
         <v>60</v>
       </c>
-      <c r="M62">
+      <c r="M67">
         <v>650</v>
       </c>
-      <c r="N62" t="s">
+      <c r="N67" t="s">
         <v>132</v>
       </c>
-      <c r="O62">
+      <c r="O67">
         <v>935539</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B63">
+      <c r="B68">
         <v>14.1412</v>
       </c>
-      <c r="C63">
+      <c r="C68">
         <v>6.5072000000000001</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D68" s="1">
         <v>9.6899999999999994E-9</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E68" s="1">
         <v>6.1855399999999996E-14</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F68" s="1">
         <v>4.1739000000000001E-5</v>
       </c>
-      <c r="G63" s="1">
+      <c r="G68" s="1">
         <v>3.3197000000000001E-4</v>
       </c>
-      <c r="H63" s="1">
+      <c r="H68" s="1">
         <v>1.0068000000000001E-4</v>
       </c>
-      <c r="I63" s="1">
+      <c r="I68" s="1">
         <f t="shared" si="1"/>
         <v>4.7438900000000003E-4</v>
       </c>
-      <c r="J63" s="3">
+      <c r="J68" s="3">
         <v>450</v>
       </c>
-      <c r="K63">
+      <c r="K68">
         <v>18</v>
       </c>
-      <c r="L63">
+      <c r="L68">
         <v>60</v>
       </c>
-      <c r="M63">
+      <c r="M68">
         <v>650</v>
       </c>
-      <c r="N63" t="s">
+      <c r="N68" t="s">
         <v>132</v>
       </c>
-      <c r="O63">
+      <c r="O68">
         <v>1038493</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B64">
+      <c r="B69">
         <v>14.1411</v>
       </c>
-      <c r="C64">
+      <c r="C69">
         <v>6.5052000000000003</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D69" s="1">
         <v>8.7799999999999999E-9</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E69" s="1">
         <v>6.8315699999999997E-14</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F69" s="1">
         <v>4.0368999999999999E-5</v>
       </c>
-      <c r="G64" s="1">
+      <c r="G69" s="1">
         <v>3.2810000000000001E-4</v>
       </c>
-      <c r="H64" s="1">
+      <c r="H69" s="1">
         <v>9.9210999999999996E-5</v>
       </c>
-      <c r="I64" s="1">
+      <c r="I69" s="1">
         <f t="shared" si="1"/>
         <v>4.6767999999999999E-4</v>
       </c>
-      <c r="J64" s="3">
+      <c r="J69" s="3">
         <v>500</v>
       </c>
-      <c r="K64">
+      <c r="K69">
         <v>18</v>
       </c>
-      <c r="L64">
+      <c r="L69">
         <v>60</v>
       </c>
-      <c r="M64">
+      <c r="M69">
         <v>650</v>
       </c>
-      <c r="N64" t="s">
+      <c r="N69" t="s">
         <v>132</v>
       </c>
-      <c r="O64">
+      <c r="O69">
         <v>1146237</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="D65" s="1"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+      <c r="D70" s="1"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B67">
+      <c r="B72">
         <v>14.141299999999999</v>
       </c>
-      <c r="C67">
+      <c r="C72">
         <v>6.5048000000000004</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D72" s="1">
         <v>9.7100000000000006E-9</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E72" s="1">
         <v>6.1720000000000001E-14</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F72" s="1">
         <v>3.7382999999999998E-5</v>
       </c>
-      <c r="G67" s="1">
+      <c r="G72" s="1">
         <v>3.0276000000000001E-4</v>
       </c>
-      <c r="H67" s="1">
+      <c r="H72" s="1">
         <v>9.5347999999999996E-5</v>
       </c>
-      <c r="I67" s="1">
-        <f>SUM(F67:H67)</f>
+      <c r="I72" s="1">
+        <f>SUM(F72:H72)</f>
         <v>4.3549099999999998E-4</v>
       </c>
-      <c r="J67">
+      <c r="J72">
         <v>450</v>
       </c>
-      <c r="K67">
+      <c r="K72">
         <v>18</v>
       </c>
-      <c r="L67">
+      <c r="L72">
         <v>60</v>
       </c>
-      <c r="M67">
+      <c r="M72">
         <v>650</v>
       </c>
-      <c r="N67" s="3">
+      <c r="N72" s="3">
         <v>5</v>
       </c>
-      <c r="O67">
+      <c r="O72">
         <v>835079</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B68">
+      <c r="B73">
         <v>14.141299999999999</v>
       </c>
-      <c r="C68">
+      <c r="C73">
         <v>6.5044000000000004</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D73" s="1">
         <v>9.7499999999999996E-9</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E73" s="1">
         <v>6.1463999999999997E-14</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F73" s="1">
         <v>3.557E-5</v>
       </c>
-      <c r="G68" s="1">
+      <c r="G73" s="1">
         <v>3.0078E-4</v>
       </c>
-      <c r="H68" s="1">
+      <c r="H73" s="1">
         <v>9.4667999999999996E-5</v>
       </c>
-      <c r="I68" s="1">
-        <f t="shared" ref="I68:I72" si="2">SUM(F68:H68)</f>
+      <c r="I73" s="1">
+        <f t="shared" ref="I73:I77" si="2">SUM(F73:H73)</f>
         <v>4.3101800000000003E-4</v>
       </c>
-      <c r="J68">
+      <c r="J73">
         <v>450</v>
       </c>
-      <c r="K68">
+      <c r="K73">
         <v>18</v>
       </c>
-      <c r="L68">
+      <c r="L73">
         <v>60</v>
       </c>
-      <c r="M68">
+      <c r="M73">
         <v>650</v>
       </c>
-      <c r="N68" s="3">
+      <c r="N73" s="3">
         <v>10</v>
       </c>
-      <c r="O68">
+      <c r="O73">
         <v>831573</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B69">
+      <c r="B74">
         <v>14.141299999999999</v>
       </c>
-      <c r="C69">
+      <c r="C74">
         <v>6.5027999999999997</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D74" s="1">
         <v>9.8099999999999998E-9</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E74" s="1">
         <v>6.1125899999999994E-14</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F74" s="1">
         <v>3.6656000000000003E-5</v>
       </c>
-      <c r="G69" s="1">
+      <c r="G74" s="1">
         <v>2.9846000000000001E-4</v>
       </c>
-      <c r="H69" s="1">
+      <c r="H74" s="1">
         <v>9.6022999999999999E-5</v>
       </c>
-      <c r="I69" s="1">
+      <c r="I74" s="1">
         <f t="shared" si="2"/>
         <v>4.3113899999999998E-4</v>
       </c>
-      <c r="J69">
+      <c r="J74">
         <v>450</v>
       </c>
-      <c r="K69">
+      <c r="K74">
         <v>18</v>
       </c>
-      <c r="L69">
+      <c r="L74">
         <v>60</v>
       </c>
-      <c r="M69">
+      <c r="M74">
         <v>650</v>
       </c>
-      <c r="N69" s="3">
+      <c r="N74" s="3">
         <v>15</v>
       </c>
-      <c r="O69">
+      <c r="O74">
         <v>824442</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B70">
+      <c r="B75">
         <v>14.141400000000001</v>
       </c>
-      <c r="C70">
+      <c r="C75">
         <v>6.5019999999999998</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D75" s="1">
         <v>9.8799999999999998E-9</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E75" s="1">
         <v>6.0706000000000002E-14</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F75" s="1">
         <v>3.3695000000000002E-5</v>
       </c>
-      <c r="G70" s="1">
+      <c r="G75" s="1">
         <v>2.9975999999999999E-4</v>
       </c>
-      <c r="H70" s="1">
+      <c r="H75" s="1">
         <v>9.5086000000000004E-5</v>
       </c>
-      <c r="I70" s="1">
+      <c r="I75" s="1">
         <f t="shared" si="2"/>
         <v>4.2854099999999995E-4</v>
       </c>
-      <c r="J70">
+      <c r="J75">
         <v>450</v>
       </c>
-      <c r="K70">
+      <c r="K75">
         <v>18</v>
       </c>
-      <c r="L70">
+      <c r="L75">
         <v>60</v>
       </c>
-      <c r="M70">
+      <c r="M75">
         <v>650</v>
       </c>
-      <c r="N70" s="3">
+      <c r="N75" s="3">
         <v>20</v>
       </c>
-      <c r="O70">
+      <c r="O75">
         <v>817046</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B71">
+      <c r="B76">
         <v>14.141299999999999</v>
       </c>
-      <c r="C71">
+      <c r="C76">
         <v>6.5255999999999998</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D76" s="1">
         <v>9.9599999999999995E-9</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E76" s="1">
         <v>6.0221000000000004E-14</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F76" s="1">
         <v>3.4653000000000002E-5</v>
       </c>
-      <c r="G71" s="1">
+      <c r="G76" s="1">
         <v>2.9682999999999999E-4</v>
       </c>
-      <c r="H71" s="1">
+      <c r="H76" s="1">
         <v>9.4098999999999995E-5</v>
       </c>
-      <c r="I71" s="1">
+      <c r="I76" s="1">
         <f t="shared" si="2"/>
         <v>4.2558199999999998E-4</v>
       </c>
-      <c r="J71">
+      <c r="J76">
         <v>450</v>
       </c>
-      <c r="K71">
+      <c r="K76">
         <v>18</v>
       </c>
-      <c r="L71">
+      <c r="L76">
         <v>60</v>
       </c>
-      <c r="M71">
+      <c r="M76">
         <v>650</v>
       </c>
-      <c r="N71" s="3">
+      <c r="N76" s="3">
         <v>25</v>
       </c>
-      <c r="O71">
+      <c r="O76">
         <v>799697</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B72">
+      <c r="B77">
         <v>14.141299999999999</v>
       </c>
-      <c r="C72">
+      <c r="C77">
         <v>6.5124000000000004</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D77" s="1">
         <v>1E-8</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E77" s="1">
         <v>5.9773400000000001E-14</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F77" s="1">
         <v>3.4888000000000002E-5</v>
       </c>
-      <c r="G72" s="1">
+      <c r="G77" s="1">
         <v>2.9881999999999999E-4</v>
       </c>
-      <c r="H72" s="1">
+      <c r="H77" s="1">
         <v>9.4730999999999998E-5</v>
       </c>
-      <c r="I72" s="1">
+      <c r="I77" s="1">
         <f t="shared" si="2"/>
         <v>4.2843899999999997E-4</v>
       </c>
-      <c r="J72">
+      <c r="J77">
         <v>450</v>
       </c>
-      <c r="K72">
+      <c r="K77">
         <v>18</v>
       </c>
-      <c r="L72">
+      <c r="L77">
         <v>60</v>
       </c>
-      <c r="M72">
+      <c r="M77">
         <v>650</v>
       </c>
-      <c r="N72" s="3">
+      <c r="N77" s="3">
         <v>29</v>
       </c>
-      <c r="O72">
+      <c r="O77">
         <v>799697</v>
       </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>154</v>
+      </c>
+      <c r="B80">
+        <v>14.1416</v>
+      </c>
+      <c r="C80">
+        <v>6.4992000000000001</v>
+      </c>
+      <c r="D80" s="1">
+        <v>9.5399999999999997E-9</v>
+      </c>
+      <c r="J80">
+        <v>450</v>
+      </c>
+      <c r="K80">
+        <v>18</v>
+      </c>
+      <c r="L80">
+        <v>60</v>
+      </c>
+      <c r="M80">
+        <v>500</v>
+      </c>
+      <c r="N80" t="s">
+        <v>132</v>
+      </c>
+      <c r="O80">
+        <v>932552</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>156</v>
+      </c>
+      <c r="B81">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C81">
+        <v>6.5052000000000003</v>
+      </c>
+      <c r="D81" s="1">
+        <v>9.6099999999999997E-9</v>
+      </c>
+      <c r="M81">
+        <v>533.33299999999997</v>
+      </c>
+      <c r="O81">
+        <v>1049051</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>155</v>
+      </c>
+      <c r="B82">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C82">
+        <v>6.5115999999999996</v>
+      </c>
+      <c r="D82" s="1">
+        <v>9.6500000000000004E-9</v>
+      </c>
+      <c r="M82" s="11">
+        <v>600</v>
+      </c>
+      <c r="O82">
+        <v>913340</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>157</v>
+      </c>
+      <c r="B83">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C83">
+        <v>6.5048000000000004</v>
+      </c>
+      <c r="D83" s="1">
+        <v>9.6699999999999999E-9</v>
+      </c>
+      <c r="M83">
+        <v>600</v>
+      </c>
+      <c r="O83">
+        <v>913529</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>158</v>
+      </c>
+      <c r="B84">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C84">
+        <v>6.5056000000000003</v>
+      </c>
+      <c r="D84" s="1">
+        <v>9.6999999999999992E-9</v>
+      </c>
+      <c r="M84">
+        <v>700</v>
+      </c>
+      <c r="O84">
+        <v>770810</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>159</v>
+      </c>
+      <c r="B85">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C85">
+        <v>6.5064000000000002</v>
+      </c>
+      <c r="D85" s="1">
+        <v>9.7100000000000006E-9</v>
+      </c>
+      <c r="M85">
+        <v>800</v>
+      </c>
+      <c r="O85">
+        <v>657293</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>161</v>
+      </c>
+      <c r="B88">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C88">
+        <v>6.5019999999999998</v>
+      </c>
+      <c r="D88" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="J88">
+        <v>329</v>
+      </c>
+      <c r="K88">
+        <v>5</v>
+      </c>
+      <c r="L88">
+        <v>60</v>
+      </c>
+      <c r="M88">
+        <v>650</v>
+      </c>
+      <c r="O88">
+        <v>713513</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>162</v>
+      </c>
+      <c r="B89">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C89">
+        <v>6.5</v>
+      </c>
+      <c r="D89" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="J89">
+        <v>381</v>
+      </c>
+      <c r="K89">
+        <v>10</v>
+      </c>
+      <c r="L89">
+        <v>60</v>
+      </c>
+      <c r="M89">
+        <v>650</v>
+      </c>
+      <c r="O89">
+        <v>860415</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>163</v>
+      </c>
+      <c r="B90">
+        <v>14.141299999999999</v>
+      </c>
+      <c r="C90">
+        <v>6.5010000000000003</v>
+      </c>
+      <c r="D90" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="J90">
+        <v>447</v>
+      </c>
+      <c r="K90">
+        <v>20</v>
+      </c>
+      <c r="L90">
+        <v>60</v>
+      </c>
+      <c r="M90">
+        <v>650</v>
+      </c>
+      <c r="O90">
+        <v>1032782</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>164</v>
+      </c>
+      <c r="B91">
+        <v>14.1412</v>
+      </c>
+      <c r="C91">
+        <v>6.5030000000000001</v>
+      </c>
+      <c r="D91" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="J91">
+        <v>554.4</v>
+      </c>
+      <c r="K91">
+        <v>50</v>
+      </c>
+      <c r="L91">
+        <v>60</v>
+      </c>
+      <c r="M91">
+        <v>650</v>
+      </c>
+      <c r="O91">
+        <v>1329796</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D92" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4625,10 +5233,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5624,6 +6232,54 @@
         <v>8.7759275103636519E-9</v>
       </c>
     </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>170</v>
+      </c>
+      <c r="B96" s="1">
+        <v>4.7172999999999999E-14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>171</v>
+      </c>
+      <c r="B97" s="1">
+        <v>5.8637900000000003E-14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>172</v>
+      </c>
+      <c r="B98" s="1">
+        <v>7.0343899999999998E-14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>173</v>
+      </c>
+      <c r="B99" s="1">
+        <v>8.2385100000000002E-14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>174</v>
+      </c>
+      <c r="B100" s="1">
+        <v>9.466854E-14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>175</v>
+      </c>
+      <c r="B101" s="1">
+        <v>1.0740223E-13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Ratio and Capacitance plots
</commit_message>
<xml_diff>
--- a/participation_ratios.xlsx
+++ b/participation_ratios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" tabRatio="582" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" tabRatio="582" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ratios" sheetId="1" r:id="rId1"/>
@@ -658,7 +658,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,12 +673,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -706,15 +700,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -724,15 +717,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="11" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4"/>
-    <xf numFmtId="11" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
-    <cellStyle name="60% - Accent5" xfId="4" builtinId="48"/>
-    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
+    <cellStyle name="Accent1" xfId="4" builtinId="29"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,11 +846,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="114020352"/>
-        <c:axId val="114021888"/>
+        <c:axId val="109756800"/>
+        <c:axId val="109758336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114020352"/>
+        <c:axId val="109756800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -869,7 +859,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114021888"/>
+        <c:crossAx val="109758336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -877,7 +867,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114021888"/>
+        <c:axId val="109758336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -888,7 +878,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114020352"/>
+        <c:crossAx val="109756800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1019,11 +1009,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="114906240"/>
-        <c:axId val="114907776"/>
+        <c:axId val="110040576"/>
+        <c:axId val="110042112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114906240"/>
+        <c:axId val="110040576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,7 +1022,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114907776"/>
+        <c:crossAx val="110042112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1040,7 +1030,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114907776"/>
+        <c:axId val="110042112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1051,7 +1041,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114906240"/>
+        <c:crossAx val="110040576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1188,11 +1178,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="114944256"/>
-        <c:axId val="114946048"/>
+        <c:axId val="110086784"/>
+        <c:axId val="110088576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114944256"/>
+        <c:axId val="110086784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1201,7 +1191,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114946048"/>
+        <c:crossAx val="110088576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1209,7 +1199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114946048"/>
+        <c:axId val="110088576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1220,7 +1210,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114944256"/>
+        <c:crossAx val="110086784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1369,11 +1359,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="114756992"/>
-        <c:axId val="114766976"/>
+        <c:axId val="82223104"/>
+        <c:axId val="82224640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114756992"/>
+        <c:axId val="82223104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1382,7 +1372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114766976"/>
+        <c:crossAx val="82224640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1390,7 +1380,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114766976"/>
+        <c:axId val="82224640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1401,7 +1391,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114756992"/>
+        <c:crossAx val="82223104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1538,11 +1528,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="114788608"/>
-        <c:axId val="114798592"/>
+        <c:axId val="101680256"/>
+        <c:axId val="101681792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114788608"/>
+        <c:axId val="101680256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,7 +1541,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114798592"/>
+        <c:crossAx val="101681792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1559,7 +1549,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114798592"/>
+        <c:axId val="101681792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,7 +1560,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114788608"/>
+        <c:crossAx val="101680256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1707,11 +1697,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115216384"/>
-        <c:axId val="115217920"/>
+        <c:axId val="109623552"/>
+        <c:axId val="109674496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115216384"/>
+        <c:axId val="109623552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1720,7 +1710,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115217920"/>
+        <c:crossAx val="109674496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1728,7 +1718,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115217920"/>
+        <c:axId val="109674496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1739,7 +1729,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115216384"/>
+        <c:crossAx val="109623552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1852,11 +1842,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115233920"/>
-        <c:axId val="115235456"/>
+        <c:axId val="109682048"/>
+        <c:axId val="101717120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115233920"/>
+        <c:axId val="109682048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1865,7 +1855,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115235456"/>
+        <c:crossAx val="101717120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1873,7 +1863,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115235456"/>
+        <c:axId val="101717120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1884,7 +1874,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115233920"/>
+        <c:crossAx val="109682048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1971,11 +1961,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115274112"/>
-        <c:axId val="115275648"/>
+        <c:axId val="101749504"/>
+        <c:axId val="101751040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115274112"/>
+        <c:axId val="101749504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1984,7 +1974,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115275648"/>
+        <c:crossAx val="101751040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1992,7 +1982,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115275648"/>
+        <c:axId val="101751040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2003,7 +1993,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115274112"/>
+        <c:crossAx val="101749504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2560,7 +2550,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,10 +2947,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="F33" sqref="F33"/>
+      <selection pane="topRight" activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3081,7 +3071,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="8" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3173,7 +3163,7 @@
         <v>4.9359999999999996E-4</v>
       </c>
       <c r="J22" s="1">
-        <f>SUM(G22:I22)</f>
+        <f t="shared" ref="J22:J29" si="0">SUM(G22:I22)</f>
         <v>2.2786999999999998E-3</v>
       </c>
       <c r="K22" s="2">
@@ -3224,7 +3214,7 @@
         <v>2.6585999999999998E-4</v>
       </c>
       <c r="J23" s="1">
-        <f>SUM(G23:I23)</f>
+        <f t="shared" si="0"/>
         <v>1.1975449999999999E-3</v>
       </c>
       <c r="K23" s="2">
@@ -3275,7 +3265,7 @@
         <v>2.6585999999999998E-4</v>
       </c>
       <c r="J24" s="1">
-        <f>SUM(G24:I24)</f>
+        <f t="shared" si="0"/>
         <v>1.1975449999999999E-3</v>
       </c>
       <c r="K24" s="2">
@@ -3326,7 +3316,7 @@
         <v>1.6066E-4</v>
       </c>
       <c r="J25" s="7">
-        <f>SUM(G25:I25)</f>
+        <f t="shared" si="0"/>
         <v>7.2434699999999997E-4</v>
       </c>
       <c r="K25" s="2">
@@ -3377,7 +3367,7 @@
         <v>1.7045999999999999E-4</v>
       </c>
       <c r="J26" s="1">
-        <f>SUM(G26:I26)</f>
+        <f t="shared" si="0"/>
         <v>7.3060099999999999E-4</v>
       </c>
       <c r="K26" s="2">
@@ -3428,7 +3418,7 @@
         <v>4.1235000000000002E-4</v>
       </c>
       <c r="J27" s="1">
-        <f>SUM(G27:I27)</f>
+        <f t="shared" si="0"/>
         <v>1.84789E-3</v>
       </c>
       <c r="K27" s="2">
@@ -3479,7 +3469,7 @@
         <v>4.4083000000000002E-4</v>
       </c>
       <c r="J28" s="1">
-        <f>SUM(G28:I28)</f>
+        <f t="shared" si="0"/>
         <v>1.9952699999999999E-3</v>
       </c>
       <c r="K28" s="2">
@@ -3530,7 +3520,7 @@
         <v>2.4617999999999998E-4</v>
       </c>
       <c r="J29" s="1">
-        <f>SUM(G29:I29)</f>
+        <f t="shared" si="0"/>
         <v>1.055086E-3</v>
       </c>
       <c r="K29" s="2">
@@ -3850,7 +3840,7 @@
       <c r="O40" s="3">
         <v>1</v>
       </c>
-      <c r="P40" s="11">
+      <c r="P40" s="9">
         <v>706509</v>
       </c>
     </row>
@@ -3877,6 +3867,10 @@
       </c>
       <c r="I41" s="1">
         <v>1.8251000000000001E-4</v>
+      </c>
+      <c r="J41" s="1">
+        <f>SUM(G41:I41)</f>
+        <v>8.4980000000000006E-4</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -4022,7 +4016,7 @@
       <c r="O44" s="3">
         <v>8</v>
       </c>
-      <c r="P44" s="11">
+      <c r="P44" s="9">
         <v>696744</v>
       </c>
     </row>
@@ -4063,23 +4057,54 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="A46" t="s">
+        <v>167</v>
+      </c>
+      <c r="B46">
+        <v>14.141400000000001</v>
+      </c>
+      <c r="C46">
+        <v>6.5324999999999998</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="E46" s="1">
+        <v>5.9999999999999997E-14</v>
+      </c>
+      <c r="F46" s="1">
+        <v>5.9993999999999997E-12</v>
+      </c>
+      <c r="G46" s="1">
+        <v>5.4271000000000003E-5</v>
+      </c>
+      <c r="H46" s="1">
+        <v>5.0586999999999995E-4</v>
+      </c>
+      <c r="I46" s="1">
+        <v>1.7045999999999999E-4</v>
+      </c>
+      <c r="J46" s="1">
+        <f t="shared" ref="J46" si="1">SUM(G46:I46)</f>
+        <v>7.3060099999999999E-4</v>
+      </c>
+      <c r="K46" s="2">
+        <v>5</v>
+      </c>
+      <c r="L46" s="4">
+        <v>20</v>
+      </c>
+      <c r="M46" s="4">
         <v>56</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="O46" s="3">
+      <c r="N46">
+        <v>20</v>
+      </c>
+      <c r="O46">
         <v>10</v>
+      </c>
+      <c r="P46">
+        <v>1.2019169999999999</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -4221,7 +4246,7 @@
       <c r="B52">
         <v>14.14</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="9">
         <v>6.6580000000000004</v>
       </c>
       <c r="E52" s="1">
@@ -4270,7 +4295,7 @@
       <c r="K53" s="2"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="8" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4405,7 +4430,7 @@
         <v>1.2769999999999999E-4</v>
       </c>
       <c r="J59" s="1">
-        <f t="shared" ref="J59:J61" si="0">SUM(G59:I59)</f>
+        <f t="shared" ref="J59:J61" si="2">SUM(G59:I59)</f>
         <v>6.0008700000000002E-4</v>
       </c>
       <c r="K59">
@@ -4451,7 +4476,7 @@
         <v>9.6681000000000005E-5</v>
       </c>
       <c r="J60" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.5773999999999999E-4</v>
       </c>
       <c r="K60">
@@ -4497,7 +4522,7 @@
         <v>7.6984999999999996E-5</v>
       </c>
       <c r="J61" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6543900000000001E-4</v>
       </c>
       <c r="K61">
@@ -4520,7 +4545,7 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="12" t="s">
+      <c r="A63" s="10" t="s">
         <v>148</v>
       </c>
     </row>
@@ -4640,7 +4665,7 @@
         <v>1.0417E-4</v>
       </c>
       <c r="J66" s="1">
-        <f t="shared" ref="J66:J69" si="1">SUM(G66:I66)</f>
+        <f t="shared" ref="J66:J69" si="3">SUM(G66:I66)</f>
         <v>4.9145500000000002E-4</v>
       </c>
       <c r="K66" s="3">
@@ -4689,7 +4714,7 @@
         <v>1.0182E-4</v>
       </c>
       <c r="J67" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.8226400000000004E-4</v>
       </c>
       <c r="K67" s="3">
@@ -4738,7 +4763,7 @@
         <v>1.0068000000000001E-4</v>
       </c>
       <c r="J68" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.7438900000000003E-4</v>
       </c>
       <c r="K68" s="3">
@@ -4787,7 +4812,7 @@
         <v>9.9210999999999996E-5</v>
       </c>
       <c r="J69" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.6767999999999999E-4</v>
       </c>
       <c r="K69" s="3">
@@ -4894,7 +4919,7 @@
         <v>9.4667999999999996E-5</v>
       </c>
       <c r="J73" s="1">
-        <f t="shared" ref="J73:J77" si="2">SUM(G73:I73)</f>
+        <f t="shared" ref="J73:J77" si="4">SUM(G73:I73)</f>
         <v>4.3101800000000003E-4</v>
       </c>
       <c r="K73">
@@ -4943,7 +4968,7 @@
         <v>9.6022999999999999E-5</v>
       </c>
       <c r="J74" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.3113899999999998E-4</v>
       </c>
       <c r="K74">
@@ -4992,7 +5017,7 @@
         <v>9.5086000000000004E-5</v>
       </c>
       <c r="J75" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.2854099999999995E-4</v>
       </c>
       <c r="K75">
@@ -5041,7 +5066,7 @@
         <v>9.4098999999999995E-5</v>
       </c>
       <c r="J76" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.2558199999999998E-4</v>
       </c>
       <c r="K76">
@@ -5090,7 +5115,7 @@
         <v>9.4730999999999998E-5</v>
       </c>
       <c r="J77" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.2843899999999997E-4</v>
       </c>
       <c r="K77">
@@ -5144,7 +5169,7 @@
         <v>9.4131999999999999E-5</v>
       </c>
       <c r="J80" s="1">
-        <f>SUM(G80:I80)</f>
+        <f t="shared" ref="J80:J85" si="5">SUM(G80:I80)</f>
         <v>4.1932199999999997E-4</v>
       </c>
       <c r="K80">
@@ -5193,7 +5218,7 @@
         <v>9.8737E-5</v>
       </c>
       <c r="J81" s="1">
-        <f>SUM(G81:I81)</f>
+        <f t="shared" si="5"/>
         <v>4.5133400000000001E-4</v>
       </c>
       <c r="N81">
@@ -5230,10 +5255,10 @@
         <v>9.6671999999999999E-5</v>
       </c>
       <c r="J82" s="1">
-        <f>SUM(G82:I82)</f>
+        <f t="shared" si="5"/>
         <v>4.4043099999999997E-4</v>
       </c>
-      <c r="N82" s="11">
+      <c r="N82" s="9">
         <v>600</v>
       </c>
       <c r="P82">
@@ -5267,7 +5292,7 @@
         <v>9.6680000000000003E-5</v>
       </c>
       <c r="J83" s="1">
-        <f>SUM(G83:I83)</f>
+        <f t="shared" si="5"/>
         <v>4.4125199999999994E-4</v>
       </c>
       <c r="N83">
@@ -5304,7 +5329,7 @@
         <v>1.0145E-4</v>
       </c>
       <c r="J84" s="1">
-        <f>SUM(G84:I84)</f>
+        <f t="shared" si="5"/>
         <v>4.4283899999999999E-4</v>
       </c>
       <c r="N84">
@@ -5341,7 +5366,7 @@
         <v>1.0730000000000001E-4</v>
       </c>
       <c r="J85" s="1">
-        <f>SUM(G85:I85)</f>
+        <f t="shared" si="5"/>
         <v>4.4601000000000005E-4</v>
       </c>
       <c r="N85">
@@ -5553,8 +5578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84:B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>